<commit_message>
add SOTUs, update index
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8F5216-931E-4939-BE79-0ECE56D79F83}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A0950A-5C01-45EA-BA46-2FD6EDA96C98}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="146">
   <si>
     <t>potusLastName</t>
   </si>
@@ -436,6 +436,36 @@
   </si>
   <si>
     <t>Thomas Jefferson, Eighth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/202933</t>
+  </si>
+  <si>
+    <t>signed "JAMES MADISON" (omitted from file)</t>
+  </si>
+  <si>
+    <t>James Madison, First Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204403</t>
+  </si>
+  <si>
+    <t>James Madison, Second Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204434</t>
+  </si>
+  <si>
+    <t>James Madison, Third Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204473</t>
+  </si>
+  <si>
+    <t>James Madison, Fourth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204504</t>
+  </si>
+  <si>
+    <t>James Madison, Fifth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204541</t>
+  </si>
+  <si>
+    <t>James Madison, Sixth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204586</t>
+  </si>
+  <si>
+    <t>James Madison, Seventh Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204622</t>
+  </si>
+  <si>
+    <t>James Madison, Eighth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/204790</t>
+  </si>
+  <si>
+    <t>word count</t>
   </si>
 </sst>
 </file>
@@ -444,7 +474,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="00"/>
+    <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -512,52 +542,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="164" formatCode="00"/>
     </dxf>
     <dxf>
       <font>
@@ -576,16 +582,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="173" formatCode="00"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -631,6 +635,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -911,15 +944,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -939,6 +970,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="00"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1496,7 +1528,1144 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>word count over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>master!$A$2:$A$234</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="233"/>
+                <c:pt idx="0">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1794</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1796</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1797</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1802</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1803</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1804</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1805</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1806</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1807</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1808</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1809</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1811</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1812</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1813</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1814</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1815</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1816</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1818</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1819</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1821</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1823</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1824</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1825</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1827</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1829</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1831</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1832</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1833</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1834</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1835</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1836</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1837</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1838</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1839</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1840</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1841</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1842</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1843</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1844</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1845</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1846</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1847</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1848</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1851</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1852</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1853</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1854</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1856</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1857</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1858</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1859</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1860</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1861</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1863</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1864</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1865</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1866</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1867</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1868</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1869</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1870</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1871</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1872</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1873</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1874</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1875</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1876</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1877</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1878</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1879</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1880</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1881</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1882</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1883</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1884</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1885</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1886</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1887</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1888</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1889</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1890</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1891</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1892</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1893</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1894</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1895</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1896</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1897</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1898</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1899</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1901</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1903</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1904</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1905</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1906</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1907</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1908</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1909</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1910</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1911</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1912</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1913</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1914</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1915</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1916</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1917</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1918</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1919</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1921</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1922</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1923</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1924</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1925</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1926</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1927</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1928</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1929</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1930</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1931</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1934</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1935</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1936</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1937</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1938</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1939</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1945</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1946</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1948</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1949</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1951</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1956</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1958</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1959</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1961</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1961</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1962</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1963</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1964</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1966</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1967</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1969</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>master!$K$2:$K$234</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="233"/>
+                <c:pt idx="0">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2314</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2920</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2879</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2218</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1505</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2203</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2271</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2101</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2932</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2868</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2681</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1833</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2449</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2273</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3249</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3264</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2114</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3146</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-771D-4A8A-B24F-6D9739640C51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="510002416"/>
+        <c:axId val="510007992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="510002416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510007992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510007992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510002416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2050,6 +3219,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2088,31 +3773,69 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2114549</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42389D5C-69E4-43C6-BAFC-19D4FE78E0E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q234" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q234" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="15" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="3">
       <calculatedColumnFormula>(A2&amp;"-"&amp;B2&amp;"-"&amp;C2&amp;"-"&amp;LOWER(D2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2423,37 +4146,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
   <dimension ref="A1:Q234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K234" activeCellId="1" sqref="A2:A234 K2:K234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.140625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" customWidth="1"/>
     <col min="15" max="15" width="26.28515625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="44.85546875" customWidth="1"/>
-    <col min="17" max="17" width="44.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2495,7 +4220,7 @@
       <c r="P1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2503,10 +4228,10 @@
       <c r="A2" s="1">
         <v>1790</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2539,16 +4264,16 @@
         <v>1790-1-8-washington.md</v>
       </c>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1790</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>12</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2581,16 +4306,16 @@
         <v>1790-12-8-washington.md</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1791</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2623,16 +4348,16 @@
         <v>1791-10-25-washington.md</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1792</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2665,16 +4390,16 @@
         <v>1792-11-6-washington.md</v>
       </c>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="7"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1793</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2707,16 +4432,16 @@
         <v>1793-12-3-washington.md</v>
       </c>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1794</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2749,16 +4474,16 @@
         <v>1794-11-19-washington.md</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1795</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="10">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2791,16 +4516,16 @@
         <v>1795-12-8-washington.md</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="7"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1796</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>12</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2833,16 +4558,16 @@
         <v>1796-12-7-washington.md</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1797</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="10">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2875,16 +4600,16 @@
         <v>1797-11-22-adams.md</v>
       </c>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1798</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="10">
         <v>12</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2917,16 +4642,16 @@
         <v>1798-12-8-adams.md</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1799</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="10">
         <v>12</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2959,16 +4684,16 @@
         <v>1799-12-3-adams.md</v>
       </c>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1800</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -3001,16 +4726,16 @@
         <v>1800-11-22-adams.md</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1801</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="10">
         <v>12</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -3043,16 +4768,16 @@
         <v>1801-12-8-jefferson.md</v>
       </c>
       <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1802</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -3085,16 +4810,16 @@
         <v>1802-12-15-jefferson.md</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1803</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="10">
         <v>10</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -3127,16 +4852,16 @@
         <v>1803-10-17-jefferson.md</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1804</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="10">
         <v>11</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -3171,7 +4896,7 @@
       <c r="P17" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" s="8" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3179,10 +4904,10 @@
       <c r="A18" s="1">
         <v>1805</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="10">
         <v>12</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -3217,7 +4942,7 @@
       <c r="P18" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="Q18" s="8" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3225,10 +4950,10 @@
       <c r="A19" s="1">
         <v>1806</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -3263,7 +4988,7 @@
       <c r="P19" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="Q19" s="8" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3271,10 +4996,10 @@
       <c r="A20" s="1">
         <v>1807</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="10">
         <v>10</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -3309,7 +5034,7 @@
       <c r="P20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="Q20" s="8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3317,10 +5042,10 @@
       <c r="A21" s="1">
         <v>1808</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="10">
         <v>11</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -3355,7 +5080,7 @@
       <c r="P21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q21" s="8" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3363,6 +5088,12 @@
       <c r="A22" s="1">
         <v>1809</v>
       </c>
+      <c r="B22" s="10">
+        <v>11</v>
+      </c>
+      <c r="C22" s="5">
+        <v>29</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
@@ -3380,7 +5111,9 @@
         <v>105</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1">
+        <v>1833</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1">
         <v>1</v>
@@ -3388,15 +5121,25 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1809---madison.md</v>
-      </c>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+        <v>1809-11-29-madison.md</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1810</v>
       </c>
+      <c r="B23" s="10">
+        <v>12</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3414,7 +5157,9 @@
         <v>105</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1">
+        <v>2449</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1">
         <v>1</v>
@@ -3422,15 +5167,25 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1810---madison.md</v>
-      </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+        <v>1810-12-5-madison.md</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1811</v>
       </c>
+      <c r="B24" s="10">
+        <v>11</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
@@ -3448,7 +5203,9 @@
         <v>105</v>
       </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="K24" s="1">
+        <v>2273</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1">
         <v>1</v>
@@ -3456,15 +5213,25 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1811---madison.md</v>
-      </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+        <v>1811-11-5-madison.md</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1812</v>
       </c>
+      <c r="B25" s="10">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>25</v>
       </c>
@@ -3482,7 +5249,9 @@
         <v>105</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1">
+        <v>3249</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
         <v>1</v>
@@ -3490,15 +5259,25 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1812---madison.md</v>
-      </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+        <v>1812-11-4-madison.md</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1813</v>
       </c>
+      <c r="B26" s="10">
+        <v>12</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3516,7 +5295,9 @@
         <v>105</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1">
+        <v>3264</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1">
         <v>2</v>
@@ -3524,15 +5305,25 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1813---madison.md</v>
-      </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+        <v>1813-12-7-madison.md</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1814</v>
       </c>
+      <c r="B27" s="10">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>25</v>
       </c>
@@ -3550,7 +5341,9 @@
         <v>105</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <v>2114</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1">
         <v>2</v>
@@ -3558,15 +5351,25 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1814---madison.md</v>
-      </c>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+        <v>1814-9-20-madison.md</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1815</v>
       </c>
+      <c r="B28" s="10">
+        <v>12</v>
+      </c>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3584,7 +5387,9 @@
         <v>105</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1">
+        <v>3146</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1">
         <v>2</v>
@@ -3592,15 +5397,25 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1815---madison.md</v>
-      </c>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+        <v>1815-12-5-madison.md</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1816</v>
       </c>
+      <c r="B29" s="10">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5">
+        <v>3</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>25</v>
       </c>
@@ -3618,7 +5433,9 @@
         <v>105</v>
       </c>
       <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+      <c r="K29" s="1">
+        <v>3367</v>
+      </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1">
         <v>2</v>
@@ -3626,10 +5443,14 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1816---madison.md</v>
-      </c>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+        <v>1816-12-3-madison.md</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -3663,7 +5484,7 @@
         <v>1817---monroe.md</v>
       </c>
       <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -3697,7 +5518,7 @@
         <v>1818---monroe.md</v>
       </c>
       <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -3731,7 +5552,7 @@
         <v>1819---monroe.md</v>
       </c>
       <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="Q32" s="7"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -3765,7 +5586,7 @@
         <v>1820---monroe.md</v>
       </c>
       <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -3799,7 +5620,7 @@
         <v>1821---monroe.md</v>
       </c>
       <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="Q34" s="7"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -3833,7 +5654,7 @@
         <v>1822---monroe.md</v>
       </c>
       <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="Q35" s="7"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -3867,7 +5688,7 @@
         <v>1823---monroe.md</v>
       </c>
       <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="Q36" s="7"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -3901,7 +5722,7 @@
         <v>1824---monroe.md</v>
       </c>
       <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
+      <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -3933,7 +5754,7 @@
         <v>1825---adams.md</v>
       </c>
       <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -3965,7 +5786,7 @@
         <v>1826---adams.md</v>
       </c>
       <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -3997,7 +5818,7 @@
         <v>1827---adams.md</v>
       </c>
       <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -4029,7 +5850,7 @@
         <v>1828---adams.md</v>
       </c>
       <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -4061,7 +5882,7 @@
         <v>1829---jackson.md</v>
       </c>
       <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
+      <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -4093,7 +5914,7 @@
         <v>1830---jackson.md</v>
       </c>
       <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -4125,7 +5946,7 @@
         <v>1831---jackson.md</v>
       </c>
       <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="Q44" s="7"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -4157,7 +5978,7 @@
         <v>1832---jackson.md</v>
       </c>
       <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -4189,7 +6010,7 @@
         <v>1833---jackson.md</v>
       </c>
       <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="Q46" s="7"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -4221,7 +6042,7 @@
         <v>1834---jackson.md</v>
       </c>
       <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="Q47" s="7"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -4253,7 +6074,7 @@
         <v>1835---jackson.md</v>
       </c>
       <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="Q48" s="7"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -4285,7 +6106,7 @@
         <v>1836---jackson.md</v>
       </c>
       <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="Q49" s="7"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -4317,7 +6138,7 @@
         <v>1837---van buren.md</v>
       </c>
       <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
+      <c r="Q50" s="7"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -4349,7 +6170,7 @@
         <v>1838---van buren.md</v>
       </c>
       <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="Q51" s="7"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
@@ -4381,7 +6202,7 @@
         <v>1839---van buren.md</v>
       </c>
       <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="Q52" s="7"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -4413,7 +6234,7 @@
         <v>1840---van buren.md</v>
       </c>
       <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
+      <c r="Q53" s="7"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
@@ -4447,7 +6268,7 @@
         <v>1841---tyler.md</v>
       </c>
       <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
+      <c r="Q54" s="7"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
@@ -4481,7 +6302,7 @@
         <v>1842---tyler.md</v>
       </c>
       <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
+      <c r="Q55" s="7"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
@@ -4515,7 +6336,7 @@
         <v>1843---tyler.md</v>
       </c>
       <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
+      <c r="Q56" s="7"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -4549,7 +6370,7 @@
         <v>1844---tyler.md</v>
       </c>
       <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
+      <c r="Q57" s="7"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
@@ -4581,7 +6402,7 @@
         <v>1845---polk.md</v>
       </c>
       <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
+      <c r="Q58" s="7"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -4613,7 +6434,7 @@
         <v>1846---polk.md</v>
       </c>
       <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
+      <c r="Q59" s="7"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -4645,7 +6466,7 @@
         <v>1847---polk.md</v>
       </c>
       <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
+      <c r="Q60" s="7"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -4677,7 +6498,7 @@
         <v>1848---polk.md</v>
       </c>
       <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
+      <c r="Q61" s="7"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -4709,7 +6530,7 @@
         <v>1849---taylor.md</v>
       </c>
       <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
+      <c r="Q62" s="7"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -4741,7 +6562,7 @@
         <v>1850---fillmore.md</v>
       </c>
       <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
+      <c r="Q63" s="7"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -4773,7 +6594,7 @@
         <v>1851---fillmore.md</v>
       </c>
       <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
+      <c r="Q64" s="7"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -4805,7 +6626,7 @@
         <v>1852---fillmore.md</v>
       </c>
       <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
+      <c r="Q65" s="7"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -4837,7 +6658,7 @@
         <v>1853---pierce.md</v>
       </c>
       <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
+      <c r="Q66" s="7"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -4869,7 +6690,7 @@
         <v>1854---pierce.md</v>
       </c>
       <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
+      <c r="Q67" s="7"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -4901,7 +6722,7 @@
         <v>1855---pierce.md</v>
       </c>
       <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
+      <c r="Q68" s="7"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -4933,7 +6754,7 @@
         <v>1856---pierce.md</v>
       </c>
       <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
+      <c r="Q69" s="7"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -4965,7 +6786,7 @@
         <v>1857---buchanan.md</v>
       </c>
       <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
+      <c r="Q70" s="7"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -4997,7 +6818,7 @@
         <v>1858---buchanan.md</v>
       </c>
       <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
+      <c r="Q71" s="7"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -5029,7 +6850,7 @@
         <v>1859---buchanan.md</v>
       </c>
       <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
+      <c r="Q72" s="7"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -5061,7 +6882,7 @@
         <v>1860---buchanan.md</v>
       </c>
       <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
+      <c r="Q73" s="7"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -5095,7 +6916,7 @@
         <v>1861---lincoln.md</v>
       </c>
       <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
+      <c r="Q74" s="7"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -5129,7 +6950,7 @@
         <v>1862---lincoln.md</v>
       </c>
       <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
+      <c r="Q75" s="7"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -5163,7 +6984,7 @@
         <v>1863---lincoln.md</v>
       </c>
       <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
+      <c r="Q76" s="7"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -5197,7 +7018,7 @@
         <v>1864---lincoln.md</v>
       </c>
       <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
+      <c r="Q77" s="7"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -5231,7 +7052,7 @@
         <v>1865---johnson.md</v>
       </c>
       <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
+      <c r="Q78" s="7"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -5265,7 +7086,7 @@
         <v>1866---johnson.md</v>
       </c>
       <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
+      <c r="Q79" s="7"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -5299,7 +7120,7 @@
         <v>1867---johnson.md</v>
       </c>
       <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
+      <c r="Q80" s="7"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
@@ -5333,7 +7154,7 @@
         <v>1868---johnson.md</v>
       </c>
       <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
+      <c r="Q81" s="7"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -5365,7 +7186,7 @@
         <v>1869---grant.md</v>
       </c>
       <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
+      <c r="Q82" s="7"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
@@ -5397,7 +7218,7 @@
         <v>1870---grant.md</v>
       </c>
       <c r="P83" s="1"/>
-      <c r="Q83" s="1"/>
+      <c r="Q83" s="7"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
@@ -5429,7 +7250,7 @@
         <v>1871---grant.md</v>
       </c>
       <c r="P84" s="1"/>
-      <c r="Q84" s="1"/>
+      <c r="Q84" s="7"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
@@ -5461,7 +7282,7 @@
         <v>1872---grant.md</v>
       </c>
       <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
+      <c r="Q85" s="7"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
@@ -5493,7 +7314,7 @@
         <v>1873---grant.md</v>
       </c>
       <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
+      <c r="Q86" s="7"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
@@ -5525,7 +7346,7 @@
         <v>1874---grant.md</v>
       </c>
       <c r="P87" s="1"/>
-      <c r="Q87" s="1"/>
+      <c r="Q87" s="7"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -5557,7 +7378,7 @@
         <v>1875---grant.md</v>
       </c>
       <c r="P88" s="1"/>
-      <c r="Q88" s="1"/>
+      <c r="Q88" s="7"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
@@ -5589,7 +7410,7 @@
         <v>1876---grant.md</v>
       </c>
       <c r="P89" s="1"/>
-      <c r="Q89" s="1"/>
+      <c r="Q89" s="7"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -5621,7 +7442,7 @@
         <v>1877---hayes.md</v>
       </c>
       <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
+      <c r="Q90" s="7"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
@@ -5653,7 +7474,7 @@
         <v>1878---hayes.md</v>
       </c>
       <c r="P91" s="1"/>
-      <c r="Q91" s="1"/>
+      <c r="Q91" s="7"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
@@ -5685,7 +7506,7 @@
         <v>1879---hayes.md</v>
       </c>
       <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
+      <c r="Q92" s="7"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
@@ -5717,7 +7538,7 @@
         <v>1880---hayes.md</v>
       </c>
       <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
+      <c r="Q93" s="7"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
@@ -5749,7 +7570,7 @@
         <v>1881---arthur.md</v>
       </c>
       <c r="P94" s="1"/>
-      <c r="Q94" s="1"/>
+      <c r="Q94" s="7"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
@@ -5781,7 +7602,7 @@
         <v>1882---arthur.md</v>
       </c>
       <c r="P95" s="1"/>
-      <c r="Q95" s="1"/>
+      <c r="Q95" s="7"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
@@ -5813,7 +7634,7 @@
         <v>1883---arthur.md</v>
       </c>
       <c r="P96" s="1"/>
-      <c r="Q96" s="1"/>
+      <c r="Q96" s="7"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
@@ -5845,7 +7666,7 @@
         <v>1884---arthur.md</v>
       </c>
       <c r="P97" s="1"/>
-      <c r="Q97" s="1"/>
+      <c r="Q97" s="7"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
@@ -5877,7 +7698,7 @@
         <v>1885---cleveland.md</v>
       </c>
       <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
+      <c r="Q98" s="7"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
@@ -5909,7 +7730,7 @@
         <v>1886---cleveland.md</v>
       </c>
       <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
+      <c r="Q99" s="7"/>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
@@ -5941,7 +7762,7 @@
         <v>1887---cleveland.md</v>
       </c>
       <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
+      <c r="Q100" s="7"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
@@ -5973,7 +7794,7 @@
         <v>1888---cleveland.md</v>
       </c>
       <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
+      <c r="Q101" s="7"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
@@ -6005,7 +7826,7 @@
         <v>1889---harrison.md</v>
       </c>
       <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
+      <c r="Q102" s="7"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
@@ -6037,7 +7858,7 @@
         <v>1890---harrison.md</v>
       </c>
       <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
+      <c r="Q103" s="7"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
@@ -6069,7 +7890,7 @@
         <v>1891---harrison.md</v>
       </c>
       <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
+      <c r="Q104" s="7"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
@@ -6101,7 +7922,7 @@
         <v>1892---harrison.md</v>
       </c>
       <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
+      <c r="Q105" s="7"/>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -6133,7 +7954,7 @@
         <v>1893---cleveland.md</v>
       </c>
       <c r="P106" s="1"/>
-      <c r="Q106" s="1"/>
+      <c r="Q106" s="7"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
@@ -6165,7 +7986,7 @@
         <v>1894---cleveland.md</v>
       </c>
       <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
+      <c r="Q107" s="7"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
@@ -6197,7 +8018,7 @@
         <v>1895---cleveland.md</v>
       </c>
       <c r="P108" s="1"/>
-      <c r="Q108" s="1"/>
+      <c r="Q108" s="7"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
@@ -6229,7 +8050,7 @@
         <v>1896---cleveland.md</v>
       </c>
       <c r="P109" s="1"/>
-      <c r="Q109" s="1"/>
+      <c r="Q109" s="7"/>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
@@ -6261,7 +8082,7 @@
         <v>1897---mckinley.md</v>
       </c>
       <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
+      <c r="Q110" s="7"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
@@ -6293,7 +8114,7 @@
         <v>1898---mckinley.md</v>
       </c>
       <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
+      <c r="Q111" s="7"/>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
@@ -6325,7 +8146,7 @@
         <v>1899---mckinley.md</v>
       </c>
       <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
+      <c r="Q112" s="7"/>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
@@ -6357,7 +8178,7 @@
         <v>1900---mckinley.md</v>
       </c>
       <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
+      <c r="Q113" s="7"/>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
@@ -6389,7 +8210,7 @@
         <v>1901---roosevelt.md</v>
       </c>
       <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
+      <c r="Q114" s="7"/>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
@@ -6421,7 +8242,7 @@
         <v>1902---roosevelt.md</v>
       </c>
       <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
+      <c r="Q115" s="7"/>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
@@ -6453,7 +8274,7 @@
         <v>1903---roosevelt.md</v>
       </c>
       <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
+      <c r="Q116" s="7"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
@@ -6485,7 +8306,7 @@
         <v>1904---roosevelt.md</v>
       </c>
       <c r="P117" s="1"/>
-      <c r="Q117" s="1"/>
+      <c r="Q117" s="7"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
@@ -6517,7 +8338,7 @@
         <v>1905---roosevelt.md</v>
       </c>
       <c r="P118" s="1"/>
-      <c r="Q118" s="1"/>
+      <c r="Q118" s="7"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -6549,7 +8370,7 @@
         <v>1906---roosevelt.md</v>
       </c>
       <c r="P119" s="1"/>
-      <c r="Q119" s="1"/>
+      <c r="Q119" s="7"/>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
@@ -6581,7 +8402,7 @@
         <v>1907---roosevelt.md</v>
       </c>
       <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
+      <c r="Q120" s="7"/>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
@@ -6613,7 +8434,7 @@
         <v>1908---roosevelt.md</v>
       </c>
       <c r="P121" s="1"/>
-      <c r="Q121" s="1"/>
+      <c r="Q121" s="7"/>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -6645,7 +8466,7 @@
         <v>1909---taft.md</v>
       </c>
       <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
+      <c r="Q122" s="7"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
@@ -6677,7 +8498,7 @@
         <v>1910---taft.md</v>
       </c>
       <c r="P123" s="1"/>
-      <c r="Q123" s="1"/>
+      <c r="Q123" s="7"/>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
@@ -6709,7 +8530,7 @@
         <v>1911---taft.md</v>
       </c>
       <c r="P124" s="1"/>
-      <c r="Q124" s="1"/>
+      <c r="Q124" s="7"/>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
@@ -6741,7 +8562,7 @@
         <v>1912---taft.md</v>
       </c>
       <c r="P125" s="1"/>
-      <c r="Q125" s="1"/>
+      <c r="Q125" s="7"/>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
@@ -6773,7 +8594,7 @@
         <v>1913---wilson.md</v>
       </c>
       <c r="P126" s="1"/>
-      <c r="Q126" s="1"/>
+      <c r="Q126" s="7"/>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
@@ -6805,7 +8626,7 @@
         <v>1914---wilson.md</v>
       </c>
       <c r="P127" s="1"/>
-      <c r="Q127" s="1"/>
+      <c r="Q127" s="7"/>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
@@ -6837,7 +8658,7 @@
         <v>1915---wilson.md</v>
       </c>
       <c r="P128" s="1"/>
-      <c r="Q128" s="1"/>
+      <c r="Q128" s="7"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
@@ -6869,7 +8690,7 @@
         <v>1916---wilson.md</v>
       </c>
       <c r="P129" s="1"/>
-      <c r="Q129" s="1"/>
+      <c r="Q129" s="7"/>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
@@ -6901,7 +8722,7 @@
         <v>1917---wilson.md</v>
       </c>
       <c r="P130" s="1"/>
-      <c r="Q130" s="1"/>
+      <c r="Q130" s="7"/>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
@@ -6933,7 +8754,7 @@
         <v>1918---wilson.md</v>
       </c>
       <c r="P131" s="1"/>
-      <c r="Q131" s="1"/>
+      <c r="Q131" s="7"/>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
@@ -6965,7 +8786,7 @@
         <v>1919---wilson.md</v>
       </c>
       <c r="P132" s="1"/>
-      <c r="Q132" s="1"/>
+      <c r="Q132" s="7"/>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
@@ -6997,7 +8818,7 @@
         <v>1920---wilson.md</v>
       </c>
       <c r="P133" s="1"/>
-      <c r="Q133" s="1"/>
+      <c r="Q133" s="7"/>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
@@ -7029,7 +8850,7 @@
         <v>1921---harding.md</v>
       </c>
       <c r="P134" s="1"/>
-      <c r="Q134" s="1"/>
+      <c r="Q134" s="7"/>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
@@ -7061,7 +8882,7 @@
         <v>1922---harding.md</v>
       </c>
       <c r="P135" s="1"/>
-      <c r="Q135" s="1"/>
+      <c r="Q135" s="7"/>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -7093,7 +8914,7 @@
         <v>1923---coolidge.md</v>
       </c>
       <c r="P136" s="1"/>
-      <c r="Q136" s="1"/>
+      <c r="Q136" s="7"/>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
@@ -7125,7 +8946,7 @@
         <v>1924---coolidge.md</v>
       </c>
       <c r="P137" s="1"/>
-      <c r="Q137" s="1"/>
+      <c r="Q137" s="7"/>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
@@ -7157,7 +8978,7 @@
         <v>1925---coolidge.md</v>
       </c>
       <c r="P138" s="1"/>
-      <c r="Q138" s="1"/>
+      <c r="Q138" s="7"/>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
@@ -7189,7 +9010,7 @@
         <v>1926---coolidge.md</v>
       </c>
       <c r="P139" s="1"/>
-      <c r="Q139" s="1"/>
+      <c r="Q139" s="7"/>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
@@ -7221,7 +9042,7 @@
         <v>1927---coolidge.md</v>
       </c>
       <c r="P140" s="1"/>
-      <c r="Q140" s="1"/>
+      <c r="Q140" s="7"/>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
@@ -7253,7 +9074,7 @@
         <v>1928---coolidge.md</v>
       </c>
       <c r="P141" s="1"/>
-      <c r="Q141" s="1"/>
+      <c r="Q141" s="7"/>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
@@ -7285,7 +9106,7 @@
         <v>1929---hoover.md</v>
       </c>
       <c r="P142" s="1"/>
-      <c r="Q142" s="1"/>
+      <c r="Q142" s="7"/>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
@@ -7317,7 +9138,7 @@
         <v>1930---hoover.md</v>
       </c>
       <c r="P143" s="1"/>
-      <c r="Q143" s="1"/>
+      <c r="Q143" s="7"/>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
@@ -7349,7 +9170,7 @@
         <v>1931---hoover.md</v>
       </c>
       <c r="P144" s="1"/>
-      <c r="Q144" s="1"/>
+      <c r="Q144" s="7"/>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
@@ -7381,7 +9202,7 @@
         <v>1932---hoover.md</v>
       </c>
       <c r="P145" s="1"/>
-      <c r="Q145" s="1"/>
+      <c r="Q145" s="7"/>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
@@ -7413,7 +9234,7 @@
         <v>1934---roosevelt.md</v>
       </c>
       <c r="P146" s="1"/>
-      <c r="Q146" s="1"/>
+      <c r="Q146" s="7"/>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
@@ -7445,7 +9266,7 @@
         <v>1935---roosevelt.md</v>
       </c>
       <c r="P147" s="1"/>
-      <c r="Q147" s="1"/>
+      <c r="Q147" s="7"/>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
@@ -7477,7 +9298,7 @@
         <v>1936---roosevelt.md</v>
       </c>
       <c r="P148" s="1"/>
-      <c r="Q148" s="1"/>
+      <c r="Q148" s="7"/>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
@@ -7509,7 +9330,7 @@
         <v>1937---roosevelt.md</v>
       </c>
       <c r="P149" s="1"/>
-      <c r="Q149" s="1"/>
+      <c r="Q149" s="7"/>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
@@ -7541,7 +9362,7 @@
         <v>1938---roosevelt.md</v>
       </c>
       <c r="P150" s="1"/>
-      <c r="Q150" s="1"/>
+      <c r="Q150" s="7"/>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
@@ -7573,7 +9394,7 @@
         <v>1939---roosevelt.md</v>
       </c>
       <c r="P151" s="1"/>
-      <c r="Q151" s="1"/>
+      <c r="Q151" s="7"/>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
@@ -7605,7 +9426,7 @@
         <v>1940---roosevelt.md</v>
       </c>
       <c r="P152" s="1"/>
-      <c r="Q152" s="1"/>
+      <c r="Q152" s="7"/>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
@@ -7637,7 +9458,7 @@
         <v>1941---roosevelt.md</v>
       </c>
       <c r="P153" s="1"/>
-      <c r="Q153" s="1"/>
+      <c r="Q153" s="7"/>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
@@ -7669,7 +9490,7 @@
         <v>1942---roosevelt.md</v>
       </c>
       <c r="P154" s="1"/>
-      <c r="Q154" s="1"/>
+      <c r="Q154" s="7"/>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
@@ -7701,7 +9522,7 @@
         <v>1943---roosevelt.md</v>
       </c>
       <c r="P155" s="1"/>
-      <c r="Q155" s="1"/>
+      <c r="Q155" s="7"/>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
@@ -7733,7 +9554,7 @@
         <v>1944---roosevelt.md</v>
       </c>
       <c r="P156" s="1"/>
-      <c r="Q156" s="1"/>
+      <c r="Q156" s="7"/>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
@@ -7767,7 +9588,7 @@
         <v>1945---roosevelt.md</v>
       </c>
       <c r="P157" s="1"/>
-      <c r="Q157" s="1"/>
+      <c r="Q157" s="7"/>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
@@ -7799,7 +9620,7 @@
         <v>1946---truman.md</v>
       </c>
       <c r="P158" s="1"/>
-      <c r="Q158" s="1"/>
+      <c r="Q158" s="7"/>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
@@ -7831,7 +9652,7 @@
         <v>1947---truman.md</v>
       </c>
       <c r="P159" s="1"/>
-      <c r="Q159" s="1"/>
+      <c r="Q159" s="7"/>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
@@ -7863,7 +9684,7 @@
         <v>1948---truman.md</v>
       </c>
       <c r="P160" s="1"/>
-      <c r="Q160" s="1"/>
+      <c r="Q160" s="7"/>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
@@ -7895,7 +9716,7 @@
         <v>1949---truman.md</v>
       </c>
       <c r="P161" s="1"/>
-      <c r="Q161" s="1"/>
+      <c r="Q161" s="7"/>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
@@ -7927,7 +9748,7 @@
         <v>1950---truman.md</v>
       </c>
       <c r="P162" s="1"/>
-      <c r="Q162" s="1"/>
+      <c r="Q162" s="7"/>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
@@ -7959,7 +9780,7 @@
         <v>1951---truman.md</v>
       </c>
       <c r="P163" s="1"/>
-      <c r="Q163" s="1"/>
+      <c r="Q163" s="7"/>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
@@ -7991,7 +9812,7 @@
         <v>1952---truman.md</v>
       </c>
       <c r="P164" s="1"/>
-      <c r="Q164" s="1"/>
+      <c r="Q164" s="7"/>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
@@ -8023,7 +9844,7 @@
         <v>1953---truman.md</v>
       </c>
       <c r="P165" s="1"/>
-      <c r="Q165" s="1"/>
+      <c r="Q165" s="7"/>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
@@ -8053,7 +9874,7 @@
         <v>1953---eisenhower.md</v>
       </c>
       <c r="P166" s="1"/>
-      <c r="Q166" s="1"/>
+      <c r="Q166" s="7"/>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
@@ -8085,7 +9906,7 @@
         <v>1954---eisenhower.md</v>
       </c>
       <c r="P167" s="1"/>
-      <c r="Q167" s="1"/>
+      <c r="Q167" s="7"/>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
@@ -8117,7 +9938,7 @@
         <v>1955---eisenhower.md</v>
       </c>
       <c r="P168" s="1"/>
-      <c r="Q168" s="1"/>
+      <c r="Q168" s="7"/>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
@@ -8151,7 +9972,7 @@
         <v>1956---eisenhower.md</v>
       </c>
       <c r="P169" s="1"/>
-      <c r="Q169" s="1"/>
+      <c r="Q169" s="7"/>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
@@ -8183,7 +10004,7 @@
         <v>1957---eisenhower.md</v>
       </c>
       <c r="P170" s="1"/>
-      <c r="Q170" s="1"/>
+      <c r="Q170" s="7"/>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
@@ -8215,7 +10036,7 @@
         <v>1958---eisenhower.md</v>
       </c>
       <c r="P171" s="1"/>
-      <c r="Q171" s="1"/>
+      <c r="Q171" s="7"/>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
@@ -8247,7 +10068,7 @@
         <v>1959---eisenhower.md</v>
       </c>
       <c r="P172" s="1"/>
-      <c r="Q172" s="1"/>
+      <c r="Q172" s="7"/>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
@@ -8279,7 +10100,7 @@
         <v>1960---eisenhower.md</v>
       </c>
       <c r="P173" s="1"/>
-      <c r="Q173" s="1"/>
+      <c r="Q173" s="7"/>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
@@ -8311,7 +10132,7 @@
         <v>1961---eisenhower.md</v>
       </c>
       <c r="P174" s="1"/>
-      <c r="Q174" s="1"/>
+      <c r="Q174" s="7"/>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
@@ -8341,7 +10162,7 @@
         <v>1961---kennedy.md</v>
       </c>
       <c r="P175" s="1"/>
-      <c r="Q175" s="1"/>
+      <c r="Q175" s="7"/>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
@@ -8373,7 +10194,7 @@
         <v>1962---kennedy.md</v>
       </c>
       <c r="P176" s="1"/>
-      <c r="Q176" s="1"/>
+      <c r="Q176" s="7"/>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
@@ -8405,7 +10226,7 @@
         <v>1963---kennedy.md</v>
       </c>
       <c r="P177" s="1"/>
-      <c r="Q177" s="1"/>
+      <c r="Q177" s="7"/>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
@@ -8437,7 +10258,7 @@
         <v>1964---johnson.md</v>
       </c>
       <c r="P178" s="1"/>
-      <c r="Q178" s="1"/>
+      <c r="Q178" s="7"/>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
@@ -8469,7 +10290,7 @@
         <v>1965---johnson.md</v>
       </c>
       <c r="P179" s="1"/>
-      <c r="Q179" s="1"/>
+      <c r="Q179" s="7"/>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
@@ -8501,7 +10322,7 @@
         <v>1966---johnson.md</v>
       </c>
       <c r="P180" s="1"/>
-      <c r="Q180" s="1"/>
+      <c r="Q180" s="7"/>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
@@ -8533,7 +10354,7 @@
         <v>1967---johnson.md</v>
       </c>
       <c r="P181" s="1"/>
-      <c r="Q181" s="1"/>
+      <c r="Q181" s="7"/>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
@@ -8565,7 +10386,7 @@
         <v>1968---johnson.md</v>
       </c>
       <c r="P182" s="1"/>
-      <c r="Q182" s="1"/>
+      <c r="Q182" s="7"/>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
@@ -8597,7 +10418,7 @@
         <v>1969---johnson.md</v>
       </c>
       <c r="P183" s="1"/>
-      <c r="Q183" s="1"/>
+      <c r="Q183" s="7"/>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
@@ -8629,7 +10450,7 @@
         <v>1970---nixon.md</v>
       </c>
       <c r="P184" s="1"/>
-      <c r="Q184" s="1"/>
+      <c r="Q184" s="7"/>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
@@ -8661,7 +10482,7 @@
         <v>1971---nixon.md</v>
       </c>
       <c r="P185" s="1"/>
-      <c r="Q185" s="1"/>
+      <c r="Q185" s="7"/>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
@@ -8693,7 +10514,7 @@
         <v>1972---nixon.md</v>
       </c>
       <c r="P186" s="1"/>
-      <c r="Q186" s="1"/>
+      <c r="Q186" s="7"/>
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
@@ -8725,7 +10546,7 @@
         <v>1972---nixon.md</v>
       </c>
       <c r="P187" s="1"/>
-      <c r="Q187" s="1"/>
+      <c r="Q187" s="7"/>
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
@@ -8759,7 +10580,7 @@
         <v>1973---nixon.md</v>
       </c>
       <c r="P188" s="1"/>
-      <c r="Q188" s="1"/>
+      <c r="Q188" s="7"/>
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
@@ -8791,7 +10612,7 @@
         <v>1974---nixon.md</v>
       </c>
       <c r="P189" s="1"/>
-      <c r="Q189" s="1"/>
+      <c r="Q189" s="7"/>
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
@@ -8823,7 +10644,7 @@
         <v>1975---ford.md</v>
       </c>
       <c r="P190" s="1"/>
-      <c r="Q190" s="1"/>
+      <c r="Q190" s="7"/>
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
@@ -8855,7 +10676,7 @@
         <v>1976---ford.md</v>
       </c>
       <c r="P191" s="1"/>
-      <c r="Q191" s="1"/>
+      <c r="Q191" s="7"/>
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
@@ -8887,7 +10708,7 @@
         <v>1977---ford.md</v>
       </c>
       <c r="P192" s="1"/>
-      <c r="Q192" s="1"/>
+      <c r="Q192" s="7"/>
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
@@ -8919,7 +10740,7 @@
         <v>1978---carter.md</v>
       </c>
       <c r="P193" s="1"/>
-      <c r="Q193" s="1"/>
+      <c r="Q193" s="7"/>
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
@@ -8951,7 +10772,7 @@
         <v>1979---carter.md</v>
       </c>
       <c r="P194" s="1"/>
-      <c r="Q194" s="1"/>
+      <c r="Q194" s="7"/>
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
@@ -8983,7 +10804,7 @@
         <v>1980---carter.md</v>
       </c>
       <c r="P195" s="1"/>
-      <c r="Q195" s="1"/>
+      <c r="Q195" s="7"/>
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
@@ -9015,7 +10836,7 @@
         <v>1981---carter.md</v>
       </c>
       <c r="P196" s="1"/>
-      <c r="Q196" s="1"/>
+      <c r="Q196" s="7"/>
     </row>
     <row r="197" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
@@ -9047,7 +10868,7 @@
         <v>1981---reagan.md</v>
       </c>
       <c r="P197" s="1"/>
-      <c r="Q197" s="1"/>
+      <c r="Q197" s="7"/>
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
@@ -9079,7 +10900,7 @@
         <v>1982---reagan.md</v>
       </c>
       <c r="P198" s="1"/>
-      <c r="Q198" s="1"/>
+      <c r="Q198" s="7"/>
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
@@ -9111,7 +10932,7 @@
         <v>1983---reagan.md</v>
       </c>
       <c r="P199" s="1"/>
-      <c r="Q199" s="1"/>
+      <c r="Q199" s="7"/>
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
@@ -9143,7 +10964,7 @@
         <v>1984---reagan.md</v>
       </c>
       <c r="P200" s="1"/>
-      <c r="Q200" s="1"/>
+      <c r="Q200" s="7"/>
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
@@ -9175,7 +10996,7 @@
         <v>1985---reagan.md</v>
       </c>
       <c r="P201" s="1"/>
-      <c r="Q201" s="1"/>
+      <c r="Q201" s="7"/>
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
@@ -9207,7 +11028,7 @@
         <v>1986---reagan.md</v>
       </c>
       <c r="P202" s="1"/>
-      <c r="Q202" s="1"/>
+      <c r="Q202" s="7"/>
     </row>
     <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
@@ -9239,7 +11060,7 @@
         <v>1987---reagan.md</v>
       </c>
       <c r="P203" s="1"/>
-      <c r="Q203" s="1"/>
+      <c r="Q203" s="7"/>
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
@@ -9271,7 +11092,7 @@
         <v>1988---reagan.md</v>
       </c>
       <c r="P204" s="1"/>
-      <c r="Q204" s="1"/>
+      <c r="Q204" s="7"/>
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
@@ -9303,7 +11124,7 @@
         <v>1989---bush.md</v>
       </c>
       <c r="P205" s="1"/>
-      <c r="Q205" s="1"/>
+      <c r="Q205" s="7"/>
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
@@ -9335,7 +11156,7 @@
         <v>1990---bush.md</v>
       </c>
       <c r="P206" s="1"/>
-      <c r="Q206" s="1"/>
+      <c r="Q206" s="7"/>
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
@@ -9365,7 +11186,7 @@
         <v>1991---bush.md</v>
       </c>
       <c r="P207" s="1"/>
-      <c r="Q207" s="1"/>
+      <c r="Q207" s="7"/>
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
@@ -9397,7 +11218,7 @@
         <v>1992---bush.md</v>
       </c>
       <c r="P208" s="1"/>
-      <c r="Q208" s="1"/>
+      <c r="Q208" s="7"/>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
@@ -9429,7 +11250,7 @@
         <v>1993---clinton.md</v>
       </c>
       <c r="P209" s="1"/>
-      <c r="Q209" s="1"/>
+      <c r="Q209" s="7"/>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
@@ -9461,7 +11282,7 @@
         <v>1994---clinton.md</v>
       </c>
       <c r="P210" s="1"/>
-      <c r="Q210" s="1"/>
+      <c r="Q210" s="7"/>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
@@ -9493,7 +11314,7 @@
         <v>1995---clinton.md</v>
       </c>
       <c r="P211" s="1"/>
-      <c r="Q211" s="1"/>
+      <c r="Q211" s="7"/>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
@@ -9525,7 +11346,7 @@
         <v>1996---clinton.md</v>
       </c>
       <c r="P212" s="1"/>
-      <c r="Q212" s="1"/>
+      <c r="Q212" s="7"/>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
@@ -9557,7 +11378,7 @@
         <v>1997---clinton.md</v>
       </c>
       <c r="P213" s="1"/>
-      <c r="Q213" s="1"/>
+      <c r="Q213" s="7"/>
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
@@ -9589,7 +11410,7 @@
         <v>1998---clinton.md</v>
       </c>
       <c r="P214" s="1"/>
-      <c r="Q214" s="1"/>
+      <c r="Q214" s="7"/>
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
@@ -9621,7 +11442,7 @@
         <v>1999---clinton.md</v>
       </c>
       <c r="P215" s="1"/>
-      <c r="Q215" s="1"/>
+      <c r="Q215" s="7"/>
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
@@ -9653,7 +11474,7 @@
         <v>2000---clinton.md</v>
       </c>
       <c r="P216" s="1"/>
-      <c r="Q216" s="1"/>
+      <c r="Q216" s="7"/>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
@@ -9685,7 +11506,7 @@
         <v>2001---bush.md</v>
       </c>
       <c r="P217" s="1"/>
-      <c r="Q217" s="1"/>
+      <c r="Q217" s="7"/>
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
@@ -9717,7 +11538,7 @@
         <v>2002---bush.md</v>
       </c>
       <c r="P218" s="1"/>
-      <c r="Q218" s="1"/>
+      <c r="Q218" s="7"/>
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
@@ -9749,7 +11570,7 @@
         <v>2003---bush.md</v>
       </c>
       <c r="P219" s="1"/>
-      <c r="Q219" s="1"/>
+      <c r="Q219" s="7"/>
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
@@ -9781,7 +11602,7 @@
         <v>2004---bush.md</v>
       </c>
       <c r="P220" s="1"/>
-      <c r="Q220" s="1"/>
+      <c r="Q220" s="7"/>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
@@ -9813,7 +11634,7 @@
         <v>2005---bush.md</v>
       </c>
       <c r="P221" s="1"/>
-      <c r="Q221" s="1"/>
+      <c r="Q221" s="7"/>
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
@@ -9845,7 +11666,7 @@
         <v>2006---bush.md</v>
       </c>
       <c r="P222" s="1"/>
-      <c r="Q222" s="1"/>
+      <c r="Q222" s="7"/>
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
@@ -9877,7 +11698,7 @@
         <v>2007---bush.md</v>
       </c>
       <c r="P223" s="1"/>
-      <c r="Q223" s="1"/>
+      <c r="Q223" s="7"/>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
@@ -9909,7 +11730,7 @@
         <v>2008---bush.md</v>
       </c>
       <c r="P224" s="1"/>
-      <c r="Q224" s="1"/>
+      <c r="Q224" s="7"/>
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
@@ -9941,7 +11762,7 @@
         <v>2009---obama.md</v>
       </c>
       <c r="P225" s="1"/>
-      <c r="Q225" s="1"/>
+      <c r="Q225" s="7"/>
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
@@ -9973,7 +11794,7 @@
         <v>2010---obama.md</v>
       </c>
       <c r="P226" s="1"/>
-      <c r="Q226" s="1"/>
+      <c r="Q226" s="7"/>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
@@ -10005,7 +11826,7 @@
         <v>2011---obama.md</v>
       </c>
       <c r="P227" s="1"/>
-      <c r="Q227" s="1"/>
+      <c r="Q227" s="7"/>
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
@@ -10037,7 +11858,7 @@
         <v>2012---obama.md</v>
       </c>
       <c r="P228" s="1"/>
-      <c r="Q228" s="1"/>
+      <c r="Q228" s="7"/>
     </row>
     <row r="229" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
@@ -10069,7 +11890,7 @@
         <v>2013---obama.md</v>
       </c>
       <c r="P229" s="1"/>
-      <c r="Q229" s="1"/>
+      <c r="Q229" s="7"/>
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
@@ -10101,9 +11922,9 @@
         <v>2014---obama.md</v>
       </c>
       <c r="P230" s="1"/>
-      <c r="Q230" s="1"/>
-    </row>
-    <row r="231" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="Q230" s="7"/>
+    </row>
+    <row r="231" spans="1:17" ht="270" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>2015</v>
       </c>
@@ -10132,10 +11953,10 @@
         <f t="shared" si="3"/>
         <v>2015---obama.md</v>
       </c>
-      <c r="P231" s="5" t="s">
+      <c r="P231" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Q231" s="4" t="s">
+      <c r="Q231" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -10169,7 +11990,7 @@
         <v>2016---obama.md</v>
       </c>
       <c r="P232" s="1"/>
-      <c r="Q232" s="1"/>
+      <c r="Q232" s="7"/>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
@@ -10201,7 +12022,7 @@
         <v>2017---trump.md</v>
       </c>
       <c r="P233" s="1"/>
-      <c r="Q233" s="1"/>
+      <c r="Q233" s="7"/>
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
@@ -10233,7 +12054,7 @@
         <v>2018---trump.md</v>
       </c>
       <c r="P234" s="1"/>
-      <c r="Q234" s="1"/>
+      <c r="Q234" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -10243,7 +12064,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B1:C1" listDataValidation="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -10311,10 +12135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DDDDA2-CD65-4F05-8376-3F7C0FDAE546}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10361,6 +12185,11 @@
       <c r="B5">
         <f>COUNTIF(Table3[deliveryMedium],vocabulary!A4)</f>
         <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add SOTUs, update toolchain with some commentary
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCAC91-01CE-4989-B96C-0351ACC8588E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16848D0A-5B4D-4BA2-9A15-7DC8150540FD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="3" r:id="rId1"/>
-    <sheet name="citations" sheetId="5" r:id="rId2"/>
-    <sheet name="stats" sheetId="4" r:id="rId3"/>
-    <sheet name="vocabulary" sheetId="2" r:id="rId4"/>
+    <sheet name="potus" sheetId="6" r:id="rId2"/>
+    <sheet name="citations" sheetId="5" r:id="rId3"/>
+    <sheet name="stats" sheetId="4" r:id="rId4"/>
+    <sheet name="vocabulary" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="182">
   <si>
     <t>potusLastName</t>
   </si>
@@ -466,6 +467,117 @@
   </si>
   <si>
     <t>word count</t>
+  </si>
+  <si>
+    <t>signed "JAMES MONROE" (omitted from file)</t>
+  </si>
+  <si>
+    <t>signed "JOHN QUINCY ADAMS" (omitted from file)</t>
+  </si>
+  <si>
+    <t>James Monroe, First Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205560</t>
+  </si>
+  <si>
+    <t>James Monroe, Second Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205598</t>
+  </si>
+  <si>
+    <t>James Monroe, Third Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205633</t>
+  </si>
+  <si>
+    <t>James Monroe, Fourth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205662</t>
+  </si>
+  <si>
+    <t>James Monroe, Fifth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205698</t>
+  </si>
+  <si>
+    <t>James Monroe, Sixth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205723</t>
+  </si>
+  <si>
+    <t>James Monroe, Seventh Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205755</t>
+  </si>
+  <si>
+    <t>James Monroe, Eighth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/205780</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>given names</t>
+  </si>
+  <si>
+    <t>year elected</t>
+  </si>
+  <si>
+    <t>date inaugurated</t>
+  </si>
+  <si>
+    <t>date left office</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>Column12</t>
+  </si>
+  <si>
+    <t>Van Buren</t>
+  </si>
+  <si>
+    <t>William Henry</t>
+  </si>
+  <si>
+    <t>John Quincy Adams, First Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/206789</t>
+  </si>
+  <si>
+    <t>John Quincy Adams, Second Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/206797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signed "JOHN QUINCY ADAMS" (omitted from file) APP Note: The following sentence was removed from the text because it appears there was an error in the recording of the document where the preceeding and succeeding sentences were partially combined into an extra sentence: "In the event of a disagreement between the commissioners, one appointed by each party, to examine and decide upon their respective claims." This change does not alter the meaning of this passage. 
+APP Note: There was a small spelling error in the document that has been corrected.
+APP Note: The phrase "and important members of the Union, which, having risen into existence" was omitted from this version of the document, but is present in other versions. We have added the phrase because its absence makes the sentence nonsensical.
+We thank Dr. Daniel W. Stowell, Independent Researcher, for his assistance identifying these errors. </t>
+  </si>
+  <si>
+    <t>John Quincy Adams, Third Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/206800</t>
+  </si>
+  <si>
+    <t>John Quincy Adams, Fourth Annual Message Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/206803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signed "JOHN QUINCY ADAMS" (omitted from file) APP Note: There is a small error in the original document. The word "department" has been changed to "kept" which makes the statement clear. We thank Dr. Daniel W. Stowell, Independent Researcher, for his assistance identifying this error. </t>
   </si>
 </sst>
 </file>
@@ -476,7 +588,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +611,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -542,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -556,12 +676,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2427,6 +2566,42 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>3367</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4432</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4376</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4709</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3462</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5856</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4760</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6426</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8433</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9089</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7836</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7056</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3815,33 +3990,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q234" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q234" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="15" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="3">
       <calculatedColumnFormula>(A2&amp;"-"&amp;B2&amp;"-"&amp;C2&amp;"-"&amp;LOWER(D2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:R46" xr:uid="{AE285793-CB7D-40A8-B930-00C5755BFACC}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{6244E28B-E0F1-47FA-8860-B6D17C3A5B62}" name="#"/>
+    <tableColumn id="2" xr3:uid="{FABE08F0-72DA-4959-98B9-7525462FEC60}" name="last name"/>
+    <tableColumn id="3" xr3:uid="{C15C58D8-E330-476F-BD7A-155EB1C4E2EF}" name="given names"/>
+    <tableColumn id="4" xr3:uid="{86B85A05-0CEA-4EE9-A990-70FE2A90F713}" name="year elected"/>
+    <tableColumn id="5" xr3:uid="{00C697A9-D213-4D34-9D8C-E755A624A319}" name="date inaugurated"/>
+    <tableColumn id="6" xr3:uid="{011C3095-0446-4782-ABA5-2D53E5961EB4}" name="date left office"/>
+    <tableColumn id="7" xr3:uid="{EEBBFEE8-8990-4C15-89AA-54868E4C814C}" name="Column1"/>
+    <tableColumn id="8" xr3:uid="{F2B68088-AF52-4782-BC1A-539A073F4DD7}" name="Column2"/>
+    <tableColumn id="9" xr3:uid="{4C020256-BCCF-42C0-89BB-0490AFF73CAE}" name="Column3"/>
+    <tableColumn id="10" xr3:uid="{A08AC827-E66E-41F8-B0ED-94440D47DA83}" name="Column4"/>
+    <tableColumn id="11" xr3:uid="{763544E1-E26C-4B65-A771-AB9DBFFE9478}" name="Column5"/>
+    <tableColumn id="12" xr3:uid="{05815270-DA49-4622-9726-B3A5CB965CC8}" name="Column6"/>
+    <tableColumn id="13" xr3:uid="{696327AA-3518-4994-BA3D-7515992A7641}" name="Column7"/>
+    <tableColumn id="14" xr3:uid="{6AD54146-B960-4C5E-9DB6-F3DB0CAAACE0}" name="Column8"/>
+    <tableColumn id="15" xr3:uid="{EE85D83F-2929-4A97-8B4F-75B321FDB4B6}" name="Column9"/>
+    <tableColumn id="16" xr3:uid="{3627664F-E9C0-43AB-BC24-6AF783A92BC5}" name="Column10"/>
+    <tableColumn id="17" xr3:uid="{56B8B592-AFAD-48CC-AC4C-C80F721B7D2E}" name="Column11"/>
+    <tableColumn id="18" xr3:uid="{615E7A3E-B05F-451E-A040-ABFCF15E4DBD}" name="Column12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F55CC327-E15B-49FD-A8D0-48E8DCA2E202}" name="Table2" displayName="Table2" ref="A1:A4" totalsRowShown="0">
   <autoFilter ref="A1:A4" xr:uid="{625CE25E-F4B4-47AF-9545-5E2E3B732498}"/>
   <tableColumns count="1">
@@ -3851,7 +4053,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{24B1097F-8F17-4E54-BDCB-4F293E4CE46B}" name="Table4" displayName="Table4" ref="C1:C8" totalsRowShown="0">
   <autoFilter ref="C1:C8" xr:uid="{6AB3AE65-9DB5-4DA4-B383-8CFF7153F508}"/>
   <tableColumns count="1">
@@ -3861,7 +4063,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8592B5D5-0084-48A4-8C72-0FDE42B50915}" name="Table5" displayName="Table5" ref="E1:E13" totalsRowShown="0">
   <autoFilter ref="E1:E13" xr:uid="{5E0E19EC-E787-4E95-B2A0-DA3101E4B9CA}"/>
   <tableColumns count="1">
@@ -3871,7 +4073,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E0C97C5F-B132-4DCF-A62A-D236753529D9}" name="Table6" displayName="Table6" ref="G1:G32" totalsRowShown="0">
   <autoFilter ref="G1:G32" xr:uid="{CB8F412D-685E-443A-B695-BC1012C614D8}"/>
   <tableColumns count="1">
@@ -4146,8 +4348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
   <dimension ref="A1:Q234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5456,6 +5658,12 @@
       <c r="A30" s="1">
         <v>1817</v>
       </c>
+      <c r="B30" s="10">
+        <v>12</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
@@ -5473,7 +5681,9 @@
         <v>105</v>
       </c>
       <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="K30" s="1">
+        <v>4432</v>
+      </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1">
         <v>1</v>
@@ -5481,15 +5691,25 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1817---monroe.md</v>
-      </c>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="7"/>
+        <v>1817-12-2-monroe.md</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1818</v>
       </c>
+      <c r="B31" s="10">
+        <v>11</v>
+      </c>
+      <c r="C31" s="5">
+        <v>16</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
@@ -5507,7 +5727,9 @@
         <v>105</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1">
+        <v>4376</v>
+      </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1">
         <v>1</v>
@@ -5515,15 +5737,25 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1818---monroe.md</v>
-      </c>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="7"/>
+        <v>1818-11-16-monroe.md</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1819</v>
       </c>
+      <c r="B32" s="10">
+        <v>12</v>
+      </c>
+      <c r="C32" s="5">
+        <v>7</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
@@ -5541,7 +5773,9 @@
         <v>105</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1">
+        <v>4709</v>
+      </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1">
         <v>1</v>
@@ -5549,15 +5783,25 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1819---monroe.md</v>
-      </c>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="7"/>
+        <v>1819-12-7-monroe.md</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1820</v>
       </c>
+      <c r="B33" s="10">
+        <v>11</v>
+      </c>
+      <c r="C33" s="5">
+        <v>14</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
@@ -5575,7 +5819,9 @@
         <v>105</v>
       </c>
       <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1">
+        <v>3462</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1">
         <v>1</v>
@@ -5583,15 +5829,25 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1820---monroe.md</v>
-      </c>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="7"/>
+        <v>1820-11-14-monroe.md</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1821</v>
       </c>
+      <c r="B34" s="10">
+        <v>12</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
@@ -5609,7 +5865,9 @@
         <v>105</v>
       </c>
       <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="K34" s="1">
+        <v>5856</v>
+      </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1">
         <v>2</v>
@@ -5617,15 +5875,25 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1821---monroe.md</v>
-      </c>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="7"/>
+        <v>1821-12-3-monroe.md</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1822</v>
       </c>
+      <c r="B35" s="10">
+        <v>12</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
@@ -5643,7 +5911,9 @@
         <v>105</v>
       </c>
       <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+      <c r="K35" s="1">
+        <v>4760</v>
+      </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1">
         <v>2</v>
@@ -5651,15 +5921,25 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1822---monroe.md</v>
-      </c>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="7"/>
+        <v>1822-12-3-monroe.md</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1823</v>
       </c>
+      <c r="B36" s="10">
+        <v>12</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
@@ -5677,7 +5957,9 @@
         <v>105</v>
       </c>
       <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="K36" s="1">
+        <v>6426</v>
+      </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1">
         <v>2</v>
@@ -5685,15 +5967,25 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1823---monroe.md</v>
-      </c>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="7"/>
+        <v>1823-12-2-monroe.md</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1824</v>
       </c>
+      <c r="B37" s="10">
+        <v>12</v>
+      </c>
+      <c r="C37" s="5">
+        <v>7</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
@@ -5711,7 +6003,9 @@
         <v>105</v>
       </c>
       <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="K37" s="1">
+        <v>8433</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1">
         <v>2</v>
@@ -5719,15 +6013,25 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1824---monroe.md</v>
-      </c>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="7"/>
+        <v>1824-12-7-monroe.md</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1825</v>
       </c>
+      <c r="B38" s="10">
+        <v>12</v>
+      </c>
+      <c r="C38" s="5">
+        <v>6</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>21</v>
       </c>
@@ -5745,21 +6049,35 @@
         <v>105</v>
       </c>
       <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="K38" s="1">
+        <v>9089</v>
+      </c>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="M38" s="1">
+        <v>1</v>
+      </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1825---adams.md</v>
-      </c>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="7"/>
+        <f>(A38&amp;"-"&amp;B38&amp;"-"&amp;C38&amp;"-"&amp;LOWER(D38)&amp;".md")</f>
+        <v>1825-12-6-adams.md</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1826</v>
       </c>
+      <c r="B39" s="10">
+        <v>12</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5</v>
+      </c>
       <c r="D39" s="1" t="s">
         <v>21</v>
       </c>
@@ -5777,21 +6095,35 @@
         <v>105</v>
       </c>
       <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
+      <c r="K39" s="1">
+        <v>7836</v>
+      </c>
       <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
+      <c r="M39" s="1">
+        <v>1</v>
+      </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1826---adams.md</v>
-      </c>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="7"/>
+        <v>1826-12-5-adams.md</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1827</v>
       </c>
+      <c r="B40" s="10">
+        <v>12</v>
+      </c>
+      <c r="C40" s="5">
+        <v>4</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>21</v>
       </c>
@@ -5809,21 +6141,35 @@
         <v>105</v>
       </c>
       <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1">
+        <v>7056</v>
+      </c>
       <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1827---adams.md</v>
-      </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="7"/>
+        <v>1827-12-4-adams.md</v>
+      </c>
+      <c r="P40" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1828</v>
       </c>
+      <c r="B41" s="10">
+        <v>12</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>21</v>
       </c>
@@ -5841,16 +6187,24 @@
         <v>105</v>
       </c>
       <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="K41" s="1">
+        <v>7397</v>
+      </c>
       <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1828---adams.md</v>
-      </c>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="7"/>
+        <v>1828-12-2-adams.md</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -12099,6 +12453,371 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204DACE3-D984-409C-96B6-E9135BF03C4B}">
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EBFBCF-E6C2-4EF0-9842-2DFDC52BE682}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -12133,7 +12852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DDDDA2-CD65-4F05-8376-3F7C0FDAE546}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -12198,7 +12917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887AFE17-B40D-4762-857E-C576C1EBAB51}">
   <dimension ref="A1:G32"/>
   <sheetViews>

</xml_diff>

<commit_message>
add reagan, bush41, clinton SOTUs
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2C05C4-B563-49F1-B9BE-6A18A7F15022}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52885C4-AB74-42BE-BE64-82DB2801E962}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="stats" sheetId="4" r:id="rId4"/>
     <sheet name="vocabulary" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="259">
   <si>
     <t>potusLastName</t>
   </si>
@@ -515,9 +515,6 @@
   </si>
   <si>
     <t>date left office</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>Column2</t>
@@ -678,6 +675,141 @@
   </si>
   <si>
     <t>George W. Bush, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/277182</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:10 p.m. in the House Chamber of the Capitol.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of Congress on Administration Goals Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/218852</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:15 p.m. in the House Chamber of the Capitol.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/219941</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:14 p.m. in the House Chamber of the Capitol.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/221902</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:14 p.m. in the House Chamber of the Capitol. The Executive order of February 13 on economy and efficiency in Government procurement through compliance with certain Immigration and Naturalization Act provisions is listed in Appendix D at the end of his volume.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/223046</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:15 p.m. in the House Chamber of the Capitol. The Executive order of September 11, 1997, establishing the American Heritage Rivers initiative was published in the Federal Register at 62 FR 48445.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/223396</t>
+  </si>
+  <si>
+    <t>Begins with the words "The President." in italics, omitted from .md file. NOTE: The President spoke at 9:12 p.m. in the House Chamber of the Capitol. In his remarks, he referred to former Senator Bob Dole and his wife, Elizabeth; and President Saddam Hussein of Iraq.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/226032</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:10 p.m. in the House Chamber of the Capitol. In his remarks, he referred to Jean Hastert, wife of Speaker J. Dennis Hastert; Evelyn M. (Lyn) Gibson, widow of Detective John M. Gibson, and Wenling Chestnut, widow of Officer Jacob J. Chestnut, whose husbands died as a result of gunshot wounds suffered during an attack at the Capitol on July 24, 1998; terrorist Usama bin Ladin, who allegedly sponsored bombing attacks on the U.S. Embassies in Kenya and Tanzania on August 7, 1998; President Saddam Hussein of Iraq; Capt. Jeffrey B. Taliaferro, USAF, Chief, Wing Weapons, 28th Operations Support Squadron, 28th Bomb Wing; and Sammy Sosa, National League Most Valuable Player in 1998.</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/230240</t>
+  </si>
+  <si>
+    <t>William J. Clinton, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/227524</t>
+  </si>
+  <si>
+    <t>NOTE: The President spoke at 9:18 p.m. in the House Chamber of the Capitol. In his remarks, he referred to Rev. Jesse Jackson, founder and president, Rainbow/PUSH Coalition; President Slobodan Milosevic of the Federal Republic of Yugoslavia (Serbia and Montenegro); President Andres Pastrana of Colombia; Pope John Paul II; and Eric Lander, director, Whitehead Institute/MIT Center for Genome Research, who spoke at the eighth White House Millennium Evening. * White House correction.</t>
+  </si>
+  <si>
+    <t>George H W</t>
+  </si>
+  <si>
+    <t>Gerald</t>
+  </si>
+  <si>
+    <t>Harry S.</t>
+  </si>
+  <si>
+    <t>Franklin D.</t>
+  </si>
+  <si>
+    <t>avg word count</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:07 p.m. in the House Chamber of the Capitol. The address was broadcast live on nationwide radio and television. The Executive order of March 12 establishing the National Commission on America's Urban Families is listed in Appendix E at the end of this volume.</t>
+  </si>
+  <si>
+    <t>George Bush, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/266921</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:09 p.m. in the House Chamber of the Capitol. He was introduced by Thomas S. Foley, Speaker of the House of Representatives. In his remarks, the President referred to Dan Quayle, President of the Senate; President Saddam Hussein of Iraq; Alan Greenspan, Chairman of the Board of Governors of the Federal Reserve System; Attorney General Dick Thornburgh; United Nations Secretary-General Javier Perez de Cuellar de la Guerra; President Mikhail Gorbachev of the Soviet Union; President Francois Mitterrand of France; President Turgut Ozal of Turkey; President Mohammed Hosni Mubarak of Egypt; President Chadli Bendjedid of Algeria; King Fahd bin Abd al-`Aziz Al Sa`ud of Saudi Arabia; King Hassan II of Morocco; Prime Minister John Major of the United Kingdom; Prime Minister Giulio Andreotti of Italy; Gen. H. Norman Schwarzkopf, commander of the U.S. forces in the Persian Gulf, and his wife, Renda; and Gen. Colin L. Powell, Chairman of the Joint Chiefs of Staff, and his wife, Alma. The address was broadcast live nationwide on radio and television. Prior to his address, the President attended a reception in the Speaker's Conference Room hosted by the congressional leadership. Parts of this address could not be verified because the tape was incomplete.</t>
+  </si>
+  <si>
+    <t>George Bush, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/265956</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:05 p.m. in the House Chamber of the Capitol. He was introduced by Thomas S. Foley, Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television. Prior to his address, the President attended a reception in the Speaker's Conference Room hosted by the congressional leadership.</t>
+  </si>
+  <si>
+    <t>George Bush, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/263819</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:07 p.m. in the House Chamber of the Capitol. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>George Bush, Address on Administration Goals Before a Joint Session of Congress Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/247737</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9 p.m. in the House Chamber at the Capitol. He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of the Congress on the Program for Economic Recovery Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/246567</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9 p.m. in the House Chamber at the Capitol. He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of the Congress Reporting on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/245636</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:03 p.m. in the House Chamber of the Capitol. He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/263103</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:02 p.m. in the House Chamber of the Capitol He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/261634</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:05 p.m. in the House Chamber of the Capitol. He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/258923</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 8:04 p.m. in the House Chamber of the Capitol. He was introduced by Thomas P. O'Neill, Jr., Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/254269</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:03 p.m. in the House Chamber of the Capitol. He was introduced by Jim Wright, Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/252758</t>
+  </si>
+  <si>
+    <t>Note: The President spoke at 9:07 p.m. in the House Chamber of the Capitol. He was introduced by Jim Wright, Speaker of the House of Representatives. The address was broadcast live on nationwide radio and television.</t>
+  </si>
+  <si>
+    <t>Ronald Reagan, Address Before a Joint Session of Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/255154</t>
   </si>
 </sst>
 </file>
@@ -769,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -783,6 +915,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -790,22 +923,7 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="00"/>
     </dxf>
     <dxf>
       <font>
@@ -824,7 +942,60 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -878,6 +1049,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -886,6 +1058,24 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -904,16 +1094,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1192,66 +1380,6 @@
           <color theme="4"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2704,6 +2832,66 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>7397</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>4571</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>5290</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>5681</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>5061</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>4310</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>3561</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>3893</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>4976</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>4917</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3879</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>4020</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>5224</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>7127</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>7547</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>9403</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>6438</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>6854</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>7436</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>7628</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>9275</c:v>
                 </c:pt>
                 <c:pt idx="215">
                   <c:v>4449</c:v>
@@ -4145,32 +4333,32 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q233" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="5"/>
     <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="3">
       <calculatedColumnFormula>(A2&amp;"-"&amp;B2&amp;"-"&amp;C2&amp;"-"&amp;LOWER(D2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:R46" xr:uid="{AE285793-CB7D-40A8-B930-00C5755BFACC}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6244E28B-E0F1-47FA-8860-B6D17C3A5B62}" name="#"/>
@@ -4179,7 +4367,7 @@
     <tableColumn id="4" xr3:uid="{86B85A05-0CEA-4EE9-A990-70FE2A90F713}" name="year elected"/>
     <tableColumn id="5" xr3:uid="{00C697A9-D213-4D34-9D8C-E755A624A319}" name="date inaugurated"/>
     <tableColumn id="6" xr3:uid="{011C3095-0446-4782-ABA5-2D53E5961EB4}" name="date left office"/>
-    <tableColumn id="7" xr3:uid="{EEBBFEE8-8990-4C15-89AA-54868E4C814C}" name="Column1"/>
+    <tableColumn id="7" xr3:uid="{EEBBFEE8-8990-4C15-89AA-54868E4C814C}" name="avg word count"/>
     <tableColumn id="8" xr3:uid="{F2B68088-AF52-4782-BC1A-539A073F4DD7}" name="Column2"/>
     <tableColumn id="9" xr3:uid="{4C020256-BCCF-42C0-89BB-0490AFF73CAE}" name="Column3"/>
     <tableColumn id="10" xr3:uid="{A08AC827-E66E-41F8-B0ED-94440D47DA83}" name="Column4"/>
@@ -4501,8 +4689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
   <dimension ref="A1:Q233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="Q235" sqref="Q235"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="M197" sqref="M197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4614,7 +4802,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1" t="str">
+      <c r="O2" s="13" t="str">
         <f>(A2&amp;"-"&amp;B2&amp;"-"&amp;C2&amp;"-"&amp;LOWER(D2)&amp;".md")</f>
         <v>1790-1-8-washington.md</v>
       </c>
@@ -4656,7 +4844,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="1" t="str">
+      <c r="O3" s="13" t="str">
         <f t="shared" ref="O3:O66" si="0">(A3&amp;"-"&amp;B3&amp;"-"&amp;C3&amp;"-"&amp;LOWER(D3)&amp;".md")</f>
         <v>1790-12-8-washington.md</v>
       </c>
@@ -4698,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="1" t="str">
+      <c r="O4" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1791-10-25-washington.md</v>
       </c>
@@ -4740,7 +4928,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1" t="str">
+      <c r="O5" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1792-11-6-washington.md</v>
       </c>
@@ -4782,7 +4970,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="1" t="str">
+      <c r="O6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1793-12-3-washington.md</v>
       </c>
@@ -4824,7 +5012,7 @@
         <v>2</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="1" t="str">
+      <c r="O7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1794-11-19-washington.md</v>
       </c>
@@ -4866,7 +5054,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1" t="str">
+      <c r="O8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1795-12-8-washington.md</v>
       </c>
@@ -4908,7 +5096,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1" t="str">
+      <c r="O9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1796-12-7-washington.md</v>
       </c>
@@ -4950,7 +5138,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="1" t="str">
+      <c r="O10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1797-11-22-adams.md</v>
       </c>
@@ -4992,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="1" t="str">
+      <c r="O11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1798-12-8-adams.md</v>
       </c>
@@ -5034,7 +5222,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="1" t="str">
+      <c r="O12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1799-12-3-adams.md</v>
       </c>
@@ -5076,7 +5264,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="1" t="str">
+      <c r="O13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1800-11-22-adams.md</v>
       </c>
@@ -5118,7 +5306,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="1"/>
-      <c r="O14" s="1" t="str">
+      <c r="O14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1801-12-8-jefferson.md</v>
       </c>
@@ -5160,7 +5348,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="1" t="str">
+      <c r="O15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1802-12-15-jefferson.md</v>
       </c>
@@ -5202,7 +5390,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="1"/>
-      <c r="O16" s="1" t="str">
+      <c r="O16" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1803-10-17-jefferson.md</v>
       </c>
@@ -5244,7 +5432,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="1"/>
-      <c r="O17" s="1" t="str">
+      <c r="O17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1804-11-8-jefferson.md</v>
       </c>
@@ -5290,7 +5478,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="1"/>
-      <c r="O18" s="1" t="str">
+      <c r="O18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1805-12-3-jefferson.md</v>
       </c>
@@ -5336,7 +5524,7 @@
         <v>2</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="1" t="str">
+      <c r="O19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1806-12-2-jefferson.md</v>
       </c>
@@ -5382,7 +5570,7 @@
         <v>2</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="1" t="str">
+      <c r="O20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1807-10-27-jefferson.md</v>
       </c>
@@ -5428,7 +5616,7 @@
         <v>2</v>
       </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1" t="str">
+      <c r="O21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1808-11-8-jefferson.md</v>
       </c>
@@ -5474,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="1" t="str">
+      <c r="O22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1809-11-29-madison.md</v>
       </c>
@@ -5520,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="1"/>
-      <c r="O23" s="1" t="str">
+      <c r="O23" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1810-12-5-madison.md</v>
       </c>
@@ -5566,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="1"/>
-      <c r="O24" s="1" t="str">
+      <c r="O24" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1811-11-5-madison.md</v>
       </c>
@@ -5612,7 +5800,7 @@
         <v>1</v>
       </c>
       <c r="N25" s="1"/>
-      <c r="O25" s="1" t="str">
+      <c r="O25" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1812-11-4-madison.md</v>
       </c>
@@ -5658,7 +5846,7 @@
         <v>2</v>
       </c>
       <c r="N26" s="1"/>
-      <c r="O26" s="1" t="str">
+      <c r="O26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1813-12-7-madison.md</v>
       </c>
@@ -5704,7 +5892,7 @@
         <v>2</v>
       </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="1" t="str">
+      <c r="O27" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1814-9-20-madison.md</v>
       </c>
@@ -5750,7 +5938,7 @@
         <v>2</v>
       </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="1" t="str">
+      <c r="O28" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1815-12-5-madison.md</v>
       </c>
@@ -5796,7 +5984,7 @@
         <v>2</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="1" t="str">
+      <c r="O29" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1816-12-3-madison.md</v>
       </c>
@@ -5842,7 +6030,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="1"/>
-      <c r="O30" s="1" t="str">
+      <c r="O30" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1817-12-2-monroe.md</v>
       </c>
@@ -5888,7 +6076,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="1" t="str">
+      <c r="O31" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1818-11-16-monroe.md</v>
       </c>
@@ -5934,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="1"/>
-      <c r="O32" s="1" t="str">
+      <c r="O32" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1819-12-7-monroe.md</v>
       </c>
@@ -5980,7 +6168,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="1" t="str">
+      <c r="O33" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1820-11-14-monroe.md</v>
       </c>
@@ -6026,7 +6214,7 @@
         <v>2</v>
       </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="1" t="str">
+      <c r="O34" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1821-12-3-monroe.md</v>
       </c>
@@ -6072,7 +6260,7 @@
         <v>2</v>
       </c>
       <c r="N35" s="1"/>
-      <c r="O35" s="1" t="str">
+      <c r="O35" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1822-12-3-monroe.md</v>
       </c>
@@ -6118,7 +6306,7 @@
         <v>2</v>
       </c>
       <c r="N36" s="1"/>
-      <c r="O36" s="1" t="str">
+      <c r="O36" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1823-12-2-monroe.md</v>
       </c>
@@ -6164,7 +6352,7 @@
         <v>2</v>
       </c>
       <c r="N37" s="1"/>
-      <c r="O37" s="1" t="str">
+      <c r="O37" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1824-12-7-monroe.md</v>
       </c>
@@ -6210,7 +6398,7 @@
         <v>1</v>
       </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="1" t="str">
+      <c r="O38" s="13" t="str">
         <f>(A38&amp;"-"&amp;B38&amp;"-"&amp;C38&amp;"-"&amp;LOWER(D38)&amp;".md")</f>
         <v>1825-12-6-adams.md</v>
       </c>
@@ -6218,7 +6406,7 @@
         <v>147</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -6256,7 +6444,7 @@
         <v>1</v>
       </c>
       <c r="N39" s="1"/>
-      <c r="O39" s="1" t="str">
+      <c r="O39" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1826-12-5-adams.md</v>
       </c>
@@ -6264,7 +6452,7 @@
         <v>147</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -6302,15 +6490,15 @@
         <v>1</v>
       </c>
       <c r="N40" s="1"/>
-      <c r="O40" s="1" t="str">
+      <c r="O40" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1827-12-4-adams.md</v>
       </c>
       <c r="P40" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q40" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -6348,15 +6536,15 @@
         <v>1</v>
       </c>
       <c r="N41" s="1"/>
-      <c r="O41" s="1" t="str">
+      <c r="O41" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1828-12-2-adams.md</v>
       </c>
       <c r="P41" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -6384,7 +6572,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="1" t="str">
+      <c r="O42" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1829---jackson.md</v>
       </c>
@@ -6416,7 +6604,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="1" t="str">
+      <c r="O43" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1830---jackson.md</v>
       </c>
@@ -6448,7 +6636,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="1" t="str">
+      <c r="O44" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1831---jackson.md</v>
       </c>
@@ -6480,7 +6668,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1" t="str">
+      <c r="O45" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1832---jackson.md</v>
       </c>
@@ -6512,7 +6700,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="1" t="str">
+      <c r="O46" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1833---jackson.md</v>
       </c>
@@ -6544,7 +6732,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="1" t="str">
+      <c r="O47" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1834---jackson.md</v>
       </c>
@@ -6576,7 +6764,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="1" t="str">
+      <c r="O48" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1835---jackson.md</v>
       </c>
@@ -6608,7 +6796,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="1" t="str">
+      <c r="O49" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1836---jackson.md</v>
       </c>
@@ -6640,7 +6828,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="1" t="str">
+      <c r="O50" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1837---van buren.md</v>
       </c>
@@ -6672,7 +6860,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="1" t="str">
+      <c r="O51" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1838---van buren.md</v>
       </c>
@@ -6704,7 +6892,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="1" t="str">
+      <c r="O52" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1839---van buren.md</v>
       </c>
@@ -6736,7 +6924,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-      <c r="O53" s="1" t="str">
+      <c r="O53" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1840---van buren.md</v>
       </c>
@@ -6770,7 +6958,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54" s="1" t="str">
+      <c r="O54" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1841---tyler.md</v>
       </c>
@@ -6804,7 +6992,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-      <c r="O55" s="1" t="str">
+      <c r="O55" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1842---tyler.md</v>
       </c>
@@ -6838,7 +7026,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="1" t="str">
+      <c r="O56" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1843---tyler.md</v>
       </c>
@@ -6872,7 +7060,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="1" t="str">
+      <c r="O57" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1844---tyler.md</v>
       </c>
@@ -6904,7 +7092,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
-      <c r="O58" s="1" t="str">
+      <c r="O58" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1845---polk.md</v>
       </c>
@@ -6936,7 +7124,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
-      <c r="O59" s="1" t="str">
+      <c r="O59" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1846---polk.md</v>
       </c>
@@ -6968,7 +7156,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="1" t="str">
+      <c r="O60" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1847---polk.md</v>
       </c>
@@ -7000,7 +7188,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
-      <c r="O61" s="1" t="str">
+      <c r="O61" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1848---polk.md</v>
       </c>
@@ -7032,7 +7220,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
-      <c r="O62" s="1" t="str">
+      <c r="O62" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1849---taylor.md</v>
       </c>
@@ -7064,7 +7252,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
-      <c r="O63" s="1" t="str">
+      <c r="O63" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1850---fillmore.md</v>
       </c>
@@ -7096,7 +7284,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
-      <c r="O64" s="1" t="str">
+      <c r="O64" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1851---fillmore.md</v>
       </c>
@@ -7128,7 +7316,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
-      <c r="O65" s="1" t="str">
+      <c r="O65" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1852---fillmore.md</v>
       </c>
@@ -7160,7 +7348,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
-      <c r="O66" s="1" t="str">
+      <c r="O66" s="13" t="str">
         <f t="shared" si="0"/>
         <v>1853---pierce.md</v>
       </c>
@@ -7192,7 +7380,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
-      <c r="O67" s="1" t="str">
+      <c r="O67" s="13" t="str">
         <f t="shared" ref="O67:O130" si="1">(A67&amp;"-"&amp;B67&amp;"-"&amp;C67&amp;"-"&amp;LOWER(D67)&amp;".md")</f>
         <v>1854---pierce.md</v>
       </c>
@@ -7224,7 +7412,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
-      <c r="O68" s="1" t="str">
+      <c r="O68" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1855---pierce.md</v>
       </c>
@@ -7256,7 +7444,7 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
-      <c r="O69" s="1" t="str">
+      <c r="O69" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1856---pierce.md</v>
       </c>
@@ -7288,7 +7476,7 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
-      <c r="O70" s="1" t="str">
+      <c r="O70" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1857---buchanan.md</v>
       </c>
@@ -7320,7 +7508,7 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
-      <c r="O71" s="1" t="str">
+      <c r="O71" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1858---buchanan.md</v>
       </c>
@@ -7352,7 +7540,7 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
-      <c r="O72" s="1" t="str">
+      <c r="O72" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1859---buchanan.md</v>
       </c>
@@ -7384,7 +7572,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
-      <c r="O73" s="1" t="str">
+      <c r="O73" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1860---buchanan.md</v>
       </c>
@@ -7418,7 +7606,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
-      <c r="O74" s="1" t="str">
+      <c r="O74" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1861---lincoln.md</v>
       </c>
@@ -7452,7 +7640,7 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
-      <c r="O75" s="1" t="str">
+      <c r="O75" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1862---lincoln.md</v>
       </c>
@@ -7486,7 +7674,7 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
-      <c r="O76" s="1" t="str">
+      <c r="O76" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1863---lincoln.md</v>
       </c>
@@ -7520,7 +7708,7 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
-      <c r="O77" s="1" t="str">
+      <c r="O77" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1864---lincoln.md</v>
       </c>
@@ -7554,7 +7742,7 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
-      <c r="O78" s="1" t="str">
+      <c r="O78" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1865---johnson.md</v>
       </c>
@@ -7588,7 +7776,7 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
-      <c r="O79" s="1" t="str">
+      <c r="O79" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1866---johnson.md</v>
       </c>
@@ -7622,7 +7810,7 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
-      <c r="O80" s="1" t="str">
+      <c r="O80" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1867---johnson.md</v>
       </c>
@@ -7656,7 +7844,7 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
-      <c r="O81" s="1" t="str">
+      <c r="O81" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1868---johnson.md</v>
       </c>
@@ -7688,7 +7876,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
-      <c r="O82" s="1" t="str">
+      <c r="O82" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1869---grant.md</v>
       </c>
@@ -7720,7 +7908,7 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
-      <c r="O83" s="1" t="str">
+      <c r="O83" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1870---grant.md</v>
       </c>
@@ -7752,7 +7940,7 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
-      <c r="O84" s="1" t="str">
+      <c r="O84" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1871---grant.md</v>
       </c>
@@ -7784,7 +7972,7 @@
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
-      <c r="O85" s="1" t="str">
+      <c r="O85" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1872---grant.md</v>
       </c>
@@ -7816,7 +8004,7 @@
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
-      <c r="O86" s="1" t="str">
+      <c r="O86" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1873---grant.md</v>
       </c>
@@ -7848,7 +8036,7 @@
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
-      <c r="O87" s="1" t="str">
+      <c r="O87" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1874---grant.md</v>
       </c>
@@ -7880,7 +8068,7 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
-      <c r="O88" s="1" t="str">
+      <c r="O88" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1875---grant.md</v>
       </c>
@@ -7912,7 +8100,7 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
-      <c r="O89" s="1" t="str">
+      <c r="O89" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1876---grant.md</v>
       </c>
@@ -7944,7 +8132,7 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
-      <c r="O90" s="1" t="str">
+      <c r="O90" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1877---hayes.md</v>
       </c>
@@ -7976,7 +8164,7 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
-      <c r="O91" s="1" t="str">
+      <c r="O91" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1878---hayes.md</v>
       </c>
@@ -8008,7 +8196,7 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
-      <c r="O92" s="1" t="str">
+      <c r="O92" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1879---hayes.md</v>
       </c>
@@ -8040,7 +8228,7 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
-      <c r="O93" s="1" t="str">
+      <c r="O93" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1880---hayes.md</v>
       </c>
@@ -8072,7 +8260,7 @@
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
-      <c r="O94" s="1" t="str">
+      <c r="O94" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1881---arthur.md</v>
       </c>
@@ -8104,7 +8292,7 @@
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
-      <c r="O95" s="1" t="str">
+      <c r="O95" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1882---arthur.md</v>
       </c>
@@ -8136,7 +8324,7 @@
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
-      <c r="O96" s="1" t="str">
+      <c r="O96" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1883---arthur.md</v>
       </c>
@@ -8168,7 +8356,7 @@
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
-      <c r="O97" s="1" t="str">
+      <c r="O97" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1884---arthur.md</v>
       </c>
@@ -8200,7 +8388,7 @@
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
-      <c r="O98" s="1" t="str">
+      <c r="O98" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1885---cleveland.md</v>
       </c>
@@ -8232,7 +8420,7 @@
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
-      <c r="O99" s="1" t="str">
+      <c r="O99" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1886---cleveland.md</v>
       </c>
@@ -8264,7 +8452,7 @@
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
-      <c r="O100" s="1" t="str">
+      <c r="O100" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1887---cleveland.md</v>
       </c>
@@ -8296,7 +8484,7 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
-      <c r="O101" s="1" t="str">
+      <c r="O101" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1888---cleveland.md</v>
       </c>
@@ -8328,7 +8516,7 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
-      <c r="O102" s="1" t="str">
+      <c r="O102" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1889---harrison.md</v>
       </c>
@@ -8360,7 +8548,7 @@
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
-      <c r="O103" s="1" t="str">
+      <c r="O103" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1890---harrison.md</v>
       </c>
@@ -8392,7 +8580,7 @@
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
-      <c r="O104" s="1" t="str">
+      <c r="O104" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1891---harrison.md</v>
       </c>
@@ -8424,7 +8612,7 @@
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
-      <c r="O105" s="1" t="str">
+      <c r="O105" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1892---harrison.md</v>
       </c>
@@ -8456,7 +8644,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
-      <c r="O106" s="1" t="str">
+      <c r="O106" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1893---cleveland.md</v>
       </c>
@@ -8488,7 +8676,7 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
-      <c r="O107" s="1" t="str">
+      <c r="O107" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1894---cleveland.md</v>
       </c>
@@ -8520,7 +8708,7 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
-      <c r="O108" s="1" t="str">
+      <c r="O108" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1895---cleveland.md</v>
       </c>
@@ -8552,7 +8740,7 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
-      <c r="O109" s="1" t="str">
+      <c r="O109" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1896---cleveland.md</v>
       </c>
@@ -8584,7 +8772,7 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
-      <c r="O110" s="1" t="str">
+      <c r="O110" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1897---mckinley.md</v>
       </c>
@@ -8616,7 +8804,7 @@
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
-      <c r="O111" s="1" t="str">
+      <c r="O111" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1898---mckinley.md</v>
       </c>
@@ -8648,7 +8836,7 @@
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
-      <c r="O112" s="1" t="str">
+      <c r="O112" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1899---mckinley.md</v>
       </c>
@@ -8680,7 +8868,7 @@
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
-      <c r="O113" s="1" t="str">
+      <c r="O113" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1900---mckinley.md</v>
       </c>
@@ -8712,7 +8900,7 @@
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
-      <c r="O114" s="1" t="str">
+      <c r="O114" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1901---roosevelt.md</v>
       </c>
@@ -8744,7 +8932,7 @@
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
-      <c r="O115" s="1" t="str">
+      <c r="O115" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1902---roosevelt.md</v>
       </c>
@@ -8776,7 +8964,7 @@
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
-      <c r="O116" s="1" t="str">
+      <c r="O116" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1903---roosevelt.md</v>
       </c>
@@ -8808,7 +8996,7 @@
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
-      <c r="O117" s="1" t="str">
+      <c r="O117" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1904---roosevelt.md</v>
       </c>
@@ -8840,7 +9028,7 @@
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
-      <c r="O118" s="1" t="str">
+      <c r="O118" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1905---roosevelt.md</v>
       </c>
@@ -8872,7 +9060,7 @@
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
-      <c r="O119" s="1" t="str">
+      <c r="O119" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1906---roosevelt.md</v>
       </c>
@@ -8904,7 +9092,7 @@
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
-      <c r="O120" s="1" t="str">
+      <c r="O120" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1907---roosevelt.md</v>
       </c>
@@ -8936,7 +9124,7 @@
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
-      <c r="O121" s="1" t="str">
+      <c r="O121" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1908---roosevelt.md</v>
       </c>
@@ -8968,7 +9156,7 @@
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
-      <c r="O122" s="1" t="str">
+      <c r="O122" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1909---taft.md</v>
       </c>
@@ -9000,7 +9188,7 @@
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
-      <c r="O123" s="1" t="str">
+      <c r="O123" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1910---taft.md</v>
       </c>
@@ -9032,7 +9220,7 @@
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
-      <c r="O124" s="1" t="str">
+      <c r="O124" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1911---taft.md</v>
       </c>
@@ -9064,7 +9252,7 @@
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
-      <c r="O125" s="1" t="str">
+      <c r="O125" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1912---taft.md</v>
       </c>
@@ -9096,7 +9284,7 @@
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
-      <c r="O126" s="1" t="str">
+      <c r="O126" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1913---wilson.md</v>
       </c>
@@ -9128,7 +9316,7 @@
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
-      <c r="O127" s="1" t="str">
+      <c r="O127" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1914---wilson.md</v>
       </c>
@@ -9160,7 +9348,7 @@
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
-      <c r="O128" s="1" t="str">
+      <c r="O128" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1915---wilson.md</v>
       </c>
@@ -9192,7 +9380,7 @@
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
-      <c r="O129" s="1" t="str">
+      <c r="O129" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1916---wilson.md</v>
       </c>
@@ -9224,7 +9412,7 @@
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
-      <c r="O130" s="1" t="str">
+      <c r="O130" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1917---wilson.md</v>
       </c>
@@ -9256,7 +9444,7 @@
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
-      <c r="O131" s="1" t="str">
+      <c r="O131" s="13" t="str">
         <f t="shared" ref="O131:O194" si="2">(A131&amp;"-"&amp;B131&amp;"-"&amp;C131&amp;"-"&amp;LOWER(D131)&amp;".md")</f>
         <v>1918---wilson.md</v>
       </c>
@@ -9288,7 +9476,7 @@
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
-      <c r="O132" s="1" t="str">
+      <c r="O132" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1919---wilson.md</v>
       </c>
@@ -9320,7 +9508,7 @@
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
-      <c r="O133" s="1" t="str">
+      <c r="O133" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1920---wilson.md</v>
       </c>
@@ -9352,7 +9540,7 @@
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
-      <c r="O134" s="1" t="str">
+      <c r="O134" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1921---harding.md</v>
       </c>
@@ -9384,7 +9572,7 @@
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
-      <c r="O135" s="1" t="str">
+      <c r="O135" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1922---harding.md</v>
       </c>
@@ -9416,7 +9604,7 @@
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
-      <c r="O136" s="1" t="str">
+      <c r="O136" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1923---coolidge.md</v>
       </c>
@@ -9448,7 +9636,7 @@
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
-      <c r="O137" s="1" t="str">
+      <c r="O137" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1924---coolidge.md</v>
       </c>
@@ -9480,7 +9668,7 @@
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
-      <c r="O138" s="1" t="str">
+      <c r="O138" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1925---coolidge.md</v>
       </c>
@@ -9512,7 +9700,7 @@
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
-      <c r="O139" s="1" t="str">
+      <c r="O139" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1926---coolidge.md</v>
       </c>
@@ -9544,7 +9732,7 @@
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
-      <c r="O140" s="1" t="str">
+      <c r="O140" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1927---coolidge.md</v>
       </c>
@@ -9576,7 +9764,7 @@
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
-      <c r="O141" s="1" t="str">
+      <c r="O141" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1928---coolidge.md</v>
       </c>
@@ -9608,7 +9796,7 @@
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
-      <c r="O142" s="1" t="str">
+      <c r="O142" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1929---hoover.md</v>
       </c>
@@ -9640,7 +9828,7 @@
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
-      <c r="O143" s="1" t="str">
+      <c r="O143" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1930---hoover.md</v>
       </c>
@@ -9672,7 +9860,7 @@
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
-      <c r="O144" s="1" t="str">
+      <c r="O144" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1931---hoover.md</v>
       </c>
@@ -9704,7 +9892,7 @@
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
-      <c r="O145" s="1" t="str">
+      <c r="O145" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1932---hoover.md</v>
       </c>
@@ -9736,7 +9924,7 @@
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
-      <c r="O146" s="1" t="str">
+      <c r="O146" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1934---roosevelt.md</v>
       </c>
@@ -9768,7 +9956,7 @@
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
-      <c r="O147" s="1" t="str">
+      <c r="O147" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1935---roosevelt.md</v>
       </c>
@@ -9800,7 +9988,7 @@
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
-      <c r="O148" s="1" t="str">
+      <c r="O148" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1936---roosevelt.md</v>
       </c>
@@ -9832,7 +10020,7 @@
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
-      <c r="O149" s="1" t="str">
+      <c r="O149" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1937---roosevelt.md</v>
       </c>
@@ -9864,7 +10052,7 @@
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
-      <c r="O150" s="1" t="str">
+      <c r="O150" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1938---roosevelt.md</v>
       </c>
@@ -9896,7 +10084,7 @@
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
-      <c r="O151" s="1" t="str">
+      <c r="O151" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1939---roosevelt.md</v>
       </c>
@@ -9928,7 +10116,7 @@
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
-      <c r="O152" s="1" t="str">
+      <c r="O152" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1940---roosevelt.md</v>
       </c>
@@ -9960,7 +10148,7 @@
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
-      <c r="O153" s="1" t="str">
+      <c r="O153" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1941---roosevelt.md</v>
       </c>
@@ -9992,7 +10180,7 @@
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
-      <c r="O154" s="1" t="str">
+      <c r="O154" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1942---roosevelt.md</v>
       </c>
@@ -10024,7 +10212,7 @@
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
-      <c r="O155" s="1" t="str">
+      <c r="O155" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1943---roosevelt.md</v>
       </c>
@@ -10056,7 +10244,7 @@
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
-      <c r="O156" s="1" t="str">
+      <c r="O156" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1944---roosevelt.md</v>
       </c>
@@ -10090,7 +10278,7 @@
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
-      <c r="O157" s="1" t="str">
+      <c r="O157" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1945---roosevelt.md</v>
       </c>
@@ -10122,7 +10310,7 @@
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
-      <c r="O158" s="1" t="str">
+      <c r="O158" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1946---truman.md</v>
       </c>
@@ -10154,7 +10342,7 @@
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
-      <c r="O159" s="1" t="str">
+      <c r="O159" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1947---truman.md</v>
       </c>
@@ -10186,7 +10374,7 @@
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
-      <c r="O160" s="1" t="str">
+      <c r="O160" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1948---truman.md</v>
       </c>
@@ -10218,7 +10406,7 @@
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
-      <c r="O161" s="1" t="str">
+      <c r="O161" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1949---truman.md</v>
       </c>
@@ -10250,7 +10438,7 @@
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
-      <c r="O162" s="1" t="str">
+      <c r="O162" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1950---truman.md</v>
       </c>
@@ -10282,7 +10470,7 @@
       <c r="L163" s="1"/>
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
-      <c r="O163" s="1" t="str">
+      <c r="O163" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1951---truman.md</v>
       </c>
@@ -10314,7 +10502,7 @@
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
-      <c r="O164" s="1" t="str">
+      <c r="O164" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1952---truman.md</v>
       </c>
@@ -10346,7 +10534,7 @@
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
-      <c r="O165" s="1" t="str">
+      <c r="O165" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1953---truman.md</v>
       </c>
@@ -10376,7 +10564,7 @@
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
-      <c r="O166" s="1" t="str">
+      <c r="O166" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1953---eisenhower.md</v>
       </c>
@@ -10408,7 +10596,7 @@
       <c r="L167" s="1"/>
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
-      <c r="O167" s="1" t="str">
+      <c r="O167" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1954---eisenhower.md</v>
       </c>
@@ -10440,7 +10628,7 @@
       <c r="L168" s="1"/>
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
-      <c r="O168" s="1" t="str">
+      <c r="O168" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1955---eisenhower.md</v>
       </c>
@@ -10474,7 +10662,7 @@
       <c r="L169" s="1"/>
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
-      <c r="O169" s="1" t="str">
+      <c r="O169" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1956---eisenhower.md</v>
       </c>
@@ -10506,7 +10694,7 @@
       <c r="L170" s="1"/>
       <c r="M170" s="1"/>
       <c r="N170" s="1"/>
-      <c r="O170" s="1" t="str">
+      <c r="O170" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1957---eisenhower.md</v>
       </c>
@@ -10538,7 +10726,7 @@
       <c r="L171" s="1"/>
       <c r="M171" s="1"/>
       <c r="N171" s="1"/>
-      <c r="O171" s="1" t="str">
+      <c r="O171" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1958---eisenhower.md</v>
       </c>
@@ -10570,7 +10758,7 @@
       <c r="L172" s="1"/>
       <c r="M172" s="1"/>
       <c r="N172" s="1"/>
-      <c r="O172" s="1" t="str">
+      <c r="O172" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1959---eisenhower.md</v>
       </c>
@@ -10602,7 +10790,7 @@
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
       <c r="N173" s="1"/>
-      <c r="O173" s="1" t="str">
+      <c r="O173" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1960---eisenhower.md</v>
       </c>
@@ -10634,7 +10822,7 @@
       <c r="L174" s="1"/>
       <c r="M174" s="1"/>
       <c r="N174" s="1"/>
-      <c r="O174" s="1" t="str">
+      <c r="O174" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1961---eisenhower.md</v>
       </c>
@@ -10664,7 +10852,7 @@
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
       <c r="N175" s="1"/>
-      <c r="O175" s="1" t="str">
+      <c r="O175" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1961---kennedy.md</v>
       </c>
@@ -10696,7 +10884,7 @@
       <c r="L176" s="1"/>
       <c r="M176" s="1"/>
       <c r="N176" s="1"/>
-      <c r="O176" s="1" t="str">
+      <c r="O176" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1962---kennedy.md</v>
       </c>
@@ -10728,7 +10916,7 @@
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
       <c r="N177" s="1"/>
-      <c r="O177" s="1" t="str">
+      <c r="O177" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1963---kennedy.md</v>
       </c>
@@ -10760,7 +10948,7 @@
       <c r="L178" s="1"/>
       <c r="M178" s="1"/>
       <c r="N178" s="1"/>
-      <c r="O178" s="1" t="str">
+      <c r="O178" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1964---johnson.md</v>
       </c>
@@ -10792,7 +10980,7 @@
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
       <c r="N179" s="1"/>
-      <c r="O179" s="1" t="str">
+      <c r="O179" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1965---johnson.md</v>
       </c>
@@ -10824,7 +11012,7 @@
       <c r="L180" s="1"/>
       <c r="M180" s="1"/>
       <c r="N180" s="1"/>
-      <c r="O180" s="1" t="str">
+      <c r="O180" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1966---johnson.md</v>
       </c>
@@ -10856,7 +11044,7 @@
       <c r="L181" s="1"/>
       <c r="M181" s="1"/>
       <c r="N181" s="1"/>
-      <c r="O181" s="1" t="str">
+      <c r="O181" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1967---johnson.md</v>
       </c>
@@ -10888,7 +11076,7 @@
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
       <c r="N182" s="1"/>
-      <c r="O182" s="1" t="str">
+      <c r="O182" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1968---johnson.md</v>
       </c>
@@ -10920,7 +11108,7 @@
       <c r="L183" s="1"/>
       <c r="M183" s="1"/>
       <c r="N183" s="1"/>
-      <c r="O183" s="1" t="str">
+      <c r="O183" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1969---johnson.md</v>
       </c>
@@ -10952,7 +11140,7 @@
       <c r="L184" s="1"/>
       <c r="M184" s="1"/>
       <c r="N184" s="1"/>
-      <c r="O184" s="1" t="str">
+      <c r="O184" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1970---nixon.md</v>
       </c>
@@ -10984,7 +11172,7 @@
       <c r="L185" s="1"/>
       <c r="M185" s="1"/>
       <c r="N185" s="1"/>
-      <c r="O185" s="1" t="str">
+      <c r="O185" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1971---nixon.md</v>
       </c>
@@ -11016,7 +11204,7 @@
       <c r="L186" s="1"/>
       <c r="M186" s="1"/>
       <c r="N186" s="1"/>
-      <c r="O186" s="1" t="str">
+      <c r="O186" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1972---nixon.md</v>
       </c>
@@ -11048,7 +11236,7 @@
       <c r="L187" s="1"/>
       <c r="M187" s="1"/>
       <c r="N187" s="1"/>
-      <c r="O187" s="1" t="str">
+      <c r="O187" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1972---nixon.md</v>
       </c>
@@ -11082,7 +11270,7 @@
       <c r="L188" s="1"/>
       <c r="M188" s="1"/>
       <c r="N188" s="1"/>
-      <c r="O188" s="1" t="str">
+      <c r="O188" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1973---nixon.md</v>
       </c>
@@ -11114,7 +11302,7 @@
       <c r="L189" s="1"/>
       <c r="M189" s="1"/>
       <c r="N189" s="1"/>
-      <c r="O189" s="1" t="str">
+      <c r="O189" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1974---nixon.md</v>
       </c>
@@ -11146,7 +11334,7 @@
       <c r="L190" s="1"/>
       <c r="M190" s="1"/>
       <c r="N190" s="1"/>
-      <c r="O190" s="1" t="str">
+      <c r="O190" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1975---ford.md</v>
       </c>
@@ -11178,7 +11366,7 @@
       <c r="L191" s="1"/>
       <c r="M191" s="1"/>
       <c r="N191" s="1"/>
-      <c r="O191" s="1" t="str">
+      <c r="O191" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1976---ford.md</v>
       </c>
@@ -11210,7 +11398,7 @@
       <c r="L192" s="1"/>
       <c r="M192" s="1"/>
       <c r="N192" s="1"/>
-      <c r="O192" s="1" t="str">
+      <c r="O192" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1977---ford.md</v>
       </c>
@@ -11242,7 +11430,7 @@
       <c r="L193" s="1"/>
       <c r="M193" s="1"/>
       <c r="N193" s="1"/>
-      <c r="O193" s="1" t="str">
+      <c r="O193" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1978---carter.md</v>
       </c>
@@ -11274,7 +11462,7 @@
       <c r="L194" s="1"/>
       <c r="M194" s="1"/>
       <c r="N194" s="1"/>
-      <c r="O194" s="1" t="str">
+      <c r="O194" s="13" t="str">
         <f t="shared" si="2"/>
         <v>1979---carter.md</v>
       </c>
@@ -11306,7 +11494,7 @@
       <c r="L195" s="1"/>
       <c r="M195" s="1"/>
       <c r="N195" s="1"/>
-      <c r="O195" s="1" t="str">
+      <c r="O195" s="13" t="str">
         <f t="shared" ref="O195:O233" si="3">(A195&amp;"-"&amp;B195&amp;"-"&amp;C195&amp;"-"&amp;LOWER(D195)&amp;".md")</f>
         <v>1980---carter.md</v>
       </c>
@@ -11338,7 +11526,7 @@
       <c r="L196" s="1"/>
       <c r="M196" s="1"/>
       <c r="N196" s="1"/>
-      <c r="O196" s="1" t="str">
+      <c r="O196" s="13" t="str">
         <f t="shared" si="3"/>
         <v>1981---carter.md</v>
       </c>
@@ -11349,6 +11537,12 @@
       <c r="A197" s="1">
         <v>1981</v>
       </c>
+      <c r="B197" s="9">
+        <v>2</v>
+      </c>
+      <c r="C197" s="4">
+        <v>18</v>
+      </c>
       <c r="D197" s="1" t="s">
         <v>15</v>
       </c>
@@ -11366,21 +11560,35 @@
         <v>108</v>
       </c>
       <c r="J197" s="1"/>
-      <c r="K197" s="1"/>
+      <c r="K197" s="1">
+        <v>4571</v>
+      </c>
       <c r="L197" s="1"/>
-      <c r="M197" s="1"/>
+      <c r="M197" s="1">
+        <v>1</v>
+      </c>
       <c r="N197" s="1"/>
-      <c r="O197" s="1" t="str">
+      <c r="O197" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1981---reagan.md</v>
-      </c>
-      <c r="P197" s="6"/>
-      <c r="Q197" s="6"/>
+        <v>1981-2-18-reagan.md</v>
+      </c>
+      <c r="P197" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q197" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>1982</v>
       </c>
+      <c r="B198" s="9">
+        <v>1</v>
+      </c>
+      <c r="C198" s="4">
+        <v>26</v>
+      </c>
       <c r="D198" s="1" t="s">
         <v>15</v>
       </c>
@@ -11398,21 +11606,35 @@
         <v>108</v>
       </c>
       <c r="J198" s="1"/>
-      <c r="K198" s="1"/>
+      <c r="K198" s="1">
+        <v>5290</v>
+      </c>
       <c r="L198" s="1"/>
-      <c r="M198" s="1"/>
+      <c r="M198" s="1">
+        <v>1</v>
+      </c>
       <c r="N198" s="1"/>
-      <c r="O198" s="1" t="str">
+      <c r="O198" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1982---reagan.md</v>
-      </c>
-      <c r="P198" s="6"/>
-      <c r="Q198" s="6"/>
+        <v>1982-1-26-reagan.md</v>
+      </c>
+      <c r="P198" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q198" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>1983</v>
       </c>
+      <c r="B199" s="9">
+        <v>1</v>
+      </c>
+      <c r="C199" s="4">
+        <v>25</v>
+      </c>
       <c r="D199" s="1" t="s">
         <v>15</v>
       </c>
@@ -11430,21 +11652,35 @@
         <v>108</v>
       </c>
       <c r="J199" s="1"/>
-      <c r="K199" s="1"/>
+      <c r="K199" s="1">
+        <v>5681</v>
+      </c>
       <c r="L199" s="1"/>
-      <c r="M199" s="1"/>
+      <c r="M199" s="1">
+        <v>1</v>
+      </c>
       <c r="N199" s="1"/>
-      <c r="O199" s="1" t="str">
+      <c r="O199" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1983---reagan.md</v>
-      </c>
-      <c r="P199" s="6"/>
-      <c r="Q199" s="6"/>
+        <v>1983-1-25-reagan.md</v>
+      </c>
+      <c r="P199" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q199" s="3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>1984</v>
       </c>
+      <c r="B200" s="9">
+        <v>1</v>
+      </c>
+      <c r="C200" s="4">
+        <v>25</v>
+      </c>
       <c r="D200" s="1" t="s">
         <v>15</v>
       </c>
@@ -11462,21 +11698,35 @@
         <v>108</v>
       </c>
       <c r="J200" s="1"/>
-      <c r="K200" s="1"/>
+      <c r="K200" s="1">
+        <v>5061</v>
+      </c>
       <c r="L200" s="1"/>
-      <c r="M200" s="1"/>
+      <c r="M200" s="1">
+        <v>1</v>
+      </c>
       <c r="N200" s="1"/>
-      <c r="O200" s="1" t="str">
+      <c r="O200" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1984---reagan.md</v>
-      </c>
-      <c r="P200" s="6"/>
-      <c r="Q200" s="6"/>
+        <v>1984-1-25-reagan.md</v>
+      </c>
+      <c r="P200" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q200" s="3" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>1985</v>
       </c>
+      <c r="B201" s="9">
+        <v>2</v>
+      </c>
+      <c r="C201" s="4">
+        <v>6</v>
+      </c>
       <c r="D201" s="1" t="s">
         <v>15</v>
       </c>
@@ -11494,21 +11744,35 @@
         <v>108</v>
       </c>
       <c r="J201" s="1"/>
-      <c r="K201" s="1"/>
+      <c r="K201" s="1">
+        <v>4310</v>
+      </c>
       <c r="L201" s="1"/>
-      <c r="M201" s="1"/>
+      <c r="M201" s="1">
+        <v>2</v>
+      </c>
       <c r="N201" s="1"/>
-      <c r="O201" s="1" t="str">
+      <c r="O201" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1985---reagan.md</v>
-      </c>
-      <c r="P201" s="6"/>
-      <c r="Q201" s="6"/>
+        <v>1985-2-6-reagan.md</v>
+      </c>
+      <c r="P201" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q201" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>1986</v>
       </c>
+      <c r="B202" s="9">
+        <v>2</v>
+      </c>
+      <c r="C202" s="4">
+        <v>4</v>
+      </c>
       <c r="D202" s="1" t="s">
         <v>15</v>
       </c>
@@ -11526,21 +11790,35 @@
         <v>108</v>
       </c>
       <c r="J202" s="1"/>
-      <c r="K202" s="1"/>
+      <c r="K202" s="1">
+        <v>3561</v>
+      </c>
       <c r="L202" s="1"/>
-      <c r="M202" s="1"/>
+      <c r="M202" s="1">
+        <v>2</v>
+      </c>
       <c r="N202" s="1"/>
-      <c r="O202" s="1" t="str">
+      <c r="O202" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1986---reagan.md</v>
-      </c>
-      <c r="P202" s="6"/>
-      <c r="Q202" s="6"/>
+        <v>1986-2-4-reagan.md</v>
+      </c>
+      <c r="P202" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q202" s="3" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>1987</v>
       </c>
+      <c r="B203" s="9">
+        <v>1</v>
+      </c>
+      <c r="C203" s="4">
+        <v>27</v>
+      </c>
       <c r="D203" s="1" t="s">
         <v>15</v>
       </c>
@@ -11558,21 +11836,35 @@
         <v>108</v>
       </c>
       <c r="J203" s="1"/>
-      <c r="K203" s="1"/>
+      <c r="K203" s="1">
+        <v>3893</v>
+      </c>
       <c r="L203" s="1"/>
-      <c r="M203" s="1"/>
+      <c r="M203" s="1">
+        <v>2</v>
+      </c>
       <c r="N203" s="1"/>
-      <c r="O203" s="1" t="str">
+      <c r="O203" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1987---reagan.md</v>
-      </c>
-      <c r="P203" s="6"/>
-      <c r="Q203" s="6"/>
+        <v>1987-1-27-reagan.md</v>
+      </c>
+      <c r="P203" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q203" s="3" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>1988</v>
       </c>
+      <c r="B204" s="9">
+        <v>1</v>
+      </c>
+      <c r="C204" s="4">
+        <v>25</v>
+      </c>
       <c r="D204" s="1" t="s">
         <v>15</v>
       </c>
@@ -11590,21 +11882,35 @@
         <v>108</v>
       </c>
       <c r="J204" s="1"/>
-      <c r="K204" s="1"/>
+      <c r="K204" s="1">
+        <v>4976</v>
+      </c>
       <c r="L204" s="1"/>
-      <c r="M204" s="1"/>
+      <c r="M204" s="1">
+        <v>2</v>
+      </c>
       <c r="N204" s="1"/>
-      <c r="O204" s="1" t="str">
+      <c r="O204" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1988---reagan.md</v>
-      </c>
-      <c r="P204" s="6"/>
-      <c r="Q204" s="6"/>
+        <v>1988-1-25-reagan.md</v>
+      </c>
+      <c r="P204" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q204" s="3" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>1989</v>
       </c>
+      <c r="B205" s="9">
+        <v>2</v>
+      </c>
+      <c r="C205" s="4">
+        <v>9</v>
+      </c>
       <c r="D205" s="1" t="s">
         <v>11</v>
       </c>
@@ -11622,21 +11928,35 @@
         <v>108</v>
       </c>
       <c r="J205" s="1"/>
-      <c r="K205" s="1"/>
+      <c r="K205" s="1">
+        <v>4917</v>
+      </c>
       <c r="L205" s="1"/>
-      <c r="M205" s="1"/>
+      <c r="M205" s="1">
+        <v>1</v>
+      </c>
       <c r="N205" s="1"/>
-      <c r="O205" s="1" t="str">
+      <c r="O205" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1989---bush.md</v>
-      </c>
-      <c r="P205" s="6"/>
-      <c r="Q205" s="6"/>
+        <v>1989-2-9-bush.md</v>
+      </c>
+      <c r="P205" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q205" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>1990</v>
       </c>
+      <c r="B206" s="9">
+        <v>1</v>
+      </c>
+      <c r="C206" s="4">
+        <v>31</v>
+      </c>
       <c r="D206" s="1" t="s">
         <v>11</v>
       </c>
@@ -11654,21 +11974,35 @@
         <v>108</v>
       </c>
       <c r="J206" s="1"/>
-      <c r="K206" s="1"/>
+      <c r="K206" s="1">
+        <v>3879</v>
+      </c>
       <c r="L206" s="1"/>
-      <c r="M206" s="1"/>
+      <c r="M206" s="1">
+        <v>1</v>
+      </c>
       <c r="N206" s="1"/>
-      <c r="O206" s="1" t="str">
+      <c r="O206" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1990---bush.md</v>
-      </c>
-      <c r="P206" s="6"/>
-      <c r="Q206" s="6"/>
+        <v>1990-1-31-bush.md</v>
+      </c>
+      <c r="P206" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q206" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>1991</v>
       </c>
+      <c r="B207" s="9">
+        <v>1</v>
+      </c>
+      <c r="C207" s="4">
+        <v>29</v>
+      </c>
       <c r="D207" s="1" t="s">
         <v>11</v>
       </c>
@@ -11679,26 +12013,42 @@
         <v>17</v>
       </c>
       <c r="G207" s="1"/>
-      <c r="H207" s="1"/>
+      <c r="H207" s="1">
+        <v>1</v>
+      </c>
       <c r="I207" s="1" t="s">
         <v>108</v>
       </c>
       <c r="J207" s="1"/>
-      <c r="K207" s="1"/>
+      <c r="K207" s="1">
+        <v>4020</v>
+      </c>
       <c r="L207" s="1"/>
-      <c r="M207" s="1"/>
+      <c r="M207" s="1">
+        <v>1</v>
+      </c>
       <c r="N207" s="1"/>
-      <c r="O207" s="1" t="str">
+      <c r="O207" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1991---bush.md</v>
-      </c>
-      <c r="P207" s="6"/>
-      <c r="Q207" s="6"/>
+        <v>1991-1-29-bush.md</v>
+      </c>
+      <c r="P207" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q207" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>1992</v>
       </c>
+      <c r="B208" s="9">
+        <v>1</v>
+      </c>
+      <c r="C208" s="4">
+        <v>28</v>
+      </c>
       <c r="D208" s="1" t="s">
         <v>11</v>
       </c>
@@ -11716,21 +12066,35 @@
         <v>108</v>
       </c>
       <c r="J208" s="1"/>
-      <c r="K208" s="1"/>
+      <c r="K208" s="1">
+        <v>5224</v>
+      </c>
       <c r="L208" s="1"/>
-      <c r="M208" s="1"/>
+      <c r="M208" s="1">
+        <v>1</v>
+      </c>
       <c r="N208" s="1"/>
-      <c r="O208" s="1" t="str">
+      <c r="O208" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1992---bush.md</v>
-      </c>
-      <c r="P208" s="6"/>
-      <c r="Q208" s="6"/>
+        <v>1992-1-28-bush.md</v>
+      </c>
+      <c r="P208" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q208" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>1993</v>
       </c>
+      <c r="B209" s="9">
+        <v>2</v>
+      </c>
+      <c r="C209" s="4">
+        <v>17</v>
+      </c>
       <c r="D209" s="1" t="s">
         <v>13</v>
       </c>
@@ -11748,21 +12112,35 @@
         <v>106</v>
       </c>
       <c r="J209" s="1"/>
-      <c r="K209" s="1"/>
+      <c r="K209" s="1">
+        <v>7127</v>
+      </c>
       <c r="L209" s="1"/>
-      <c r="M209" s="1"/>
+      <c r="M209" s="1">
+        <v>1</v>
+      </c>
       <c r="N209" s="1"/>
-      <c r="O209" s="1" t="str">
+      <c r="O209" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1993---clinton.md</v>
-      </c>
-      <c r="P209" s="6"/>
-      <c r="Q209" s="6"/>
+        <v>1993-2-17-clinton.md</v>
+      </c>
+      <c r="P209" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q209" s="3" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>1994</v>
       </c>
+      <c r="B210" s="9">
+        <v>1</v>
+      </c>
+      <c r="C210" s="4">
+        <v>25</v>
+      </c>
       <c r="D210" s="1" t="s">
         <v>13</v>
       </c>
@@ -11780,21 +12158,35 @@
         <v>106</v>
       </c>
       <c r="J210" s="1"/>
-      <c r="K210" s="1"/>
+      <c r="K210" s="1">
+        <v>7547</v>
+      </c>
       <c r="L210" s="1"/>
-      <c r="M210" s="1"/>
+      <c r="M210" s="1">
+        <v>1</v>
+      </c>
       <c r="N210" s="1"/>
-      <c r="O210" s="1" t="str">
+      <c r="O210" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1994---clinton.md</v>
-      </c>
-      <c r="P210" s="6"/>
-      <c r="Q210" s="6"/>
+        <v>1994-1-25-clinton.md</v>
+      </c>
+      <c r="P210" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q210" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>1995</v>
       </c>
+      <c r="B211" s="9">
+        <v>1</v>
+      </c>
+      <c r="C211" s="4">
+        <v>24</v>
+      </c>
       <c r="D211" s="1" t="s">
         <v>13</v>
       </c>
@@ -11812,21 +12204,35 @@
         <v>106</v>
       </c>
       <c r="J211" s="1"/>
-      <c r="K211" s="1"/>
+      <c r="K211" s="1">
+        <v>9403</v>
+      </c>
       <c r="L211" s="1"/>
-      <c r="M211" s="1"/>
+      <c r="M211" s="1">
+        <v>1</v>
+      </c>
       <c r="N211" s="1"/>
-      <c r="O211" s="1" t="str">
+      <c r="O211" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1995---clinton.md</v>
-      </c>
-      <c r="P211" s="6"/>
-      <c r="Q211" s="6"/>
+        <v>1995-1-24-clinton.md</v>
+      </c>
+      <c r="P211" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q211" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>1996</v>
       </c>
+      <c r="B212" s="9">
+        <v>1</v>
+      </c>
+      <c r="C212" s="4">
+        <v>23</v>
+      </c>
       <c r="D212" s="1" t="s">
         <v>13</v>
       </c>
@@ -11844,21 +12250,35 @@
         <v>106</v>
       </c>
       <c r="J212" s="1"/>
-      <c r="K212" s="1"/>
+      <c r="K212" s="1">
+        <v>6438</v>
+      </c>
       <c r="L212" s="1"/>
-      <c r="M212" s="1"/>
+      <c r="M212" s="1">
+        <v>1</v>
+      </c>
       <c r="N212" s="1"/>
-      <c r="O212" s="1" t="str">
+      <c r="O212" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1996---clinton.md</v>
-      </c>
-      <c r="P212" s="6"/>
-      <c r="Q212" s="6"/>
+        <v>1996-1-23-clinton.md</v>
+      </c>
+      <c r="P212" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q212" s="3" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>1997</v>
       </c>
+      <c r="B213" s="9">
+        <v>2</v>
+      </c>
+      <c r="C213" s="4">
+        <v>4</v>
+      </c>
       <c r="D213" s="1" t="s">
         <v>13</v>
       </c>
@@ -11876,21 +12296,35 @@
         <v>106</v>
       </c>
       <c r="J213" s="1"/>
-      <c r="K213" s="1"/>
+      <c r="K213" s="1">
+        <v>6854</v>
+      </c>
       <c r="L213" s="1"/>
-      <c r="M213" s="1"/>
+      <c r="M213" s="1">
+        <v>2</v>
+      </c>
       <c r="N213" s="1"/>
-      <c r="O213" s="1" t="str">
+      <c r="O213" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1997---clinton.md</v>
-      </c>
-      <c r="P213" s="6"/>
-      <c r="Q213" s="6"/>
+        <v>1997-2-4-clinton.md</v>
+      </c>
+      <c r="P213" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q213" s="3" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>1998</v>
       </c>
+      <c r="B214" s="9">
+        <v>1</v>
+      </c>
+      <c r="C214" s="4">
+        <v>27</v>
+      </c>
       <c r="D214" s="1" t="s">
         <v>13</v>
       </c>
@@ -11908,21 +12342,35 @@
         <v>106</v>
       </c>
       <c r="J214" s="1"/>
-      <c r="K214" s="1"/>
+      <c r="K214" s="1">
+        <v>7436</v>
+      </c>
       <c r="L214" s="1"/>
-      <c r="M214" s="1"/>
+      <c r="M214" s="1">
+        <v>2</v>
+      </c>
       <c r="N214" s="1"/>
-      <c r="O214" s="1" t="str">
+      <c r="O214" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1998---clinton.md</v>
-      </c>
-      <c r="P214" s="6"/>
-      <c r="Q214" s="6"/>
+        <v>1998-1-27-clinton.md</v>
+      </c>
+      <c r="P214" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q214" s="3" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>1999</v>
       </c>
+      <c r="B215" s="9">
+        <v>1</v>
+      </c>
+      <c r="C215" s="4">
+        <v>19</v>
+      </c>
       <c r="D215" s="1" t="s">
         <v>13</v>
       </c>
@@ -11940,21 +12388,35 @@
         <v>106</v>
       </c>
       <c r="J215" s="1"/>
-      <c r="K215" s="1"/>
+      <c r="K215" s="1">
+        <v>7628</v>
+      </c>
       <c r="L215" s="1"/>
-      <c r="M215" s="1"/>
+      <c r="M215" s="1">
+        <v>2</v>
+      </c>
       <c r="N215" s="1"/>
-      <c r="O215" s="1" t="str">
+      <c r="O215" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>1999---clinton.md</v>
-      </c>
-      <c r="P215" s="6"/>
-      <c r="Q215" s="6"/>
+        <v>1999-1-19-clinton.md</v>
+      </c>
+      <c r="P215" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q215" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2000</v>
       </c>
+      <c r="B216" s="9">
+        <v>1</v>
+      </c>
+      <c r="C216" s="4">
+        <v>27</v>
+      </c>
       <c r="D216" s="1" t="s">
         <v>13</v>
       </c>
@@ -11972,16 +12434,24 @@
         <v>106</v>
       </c>
       <c r="J216" s="1"/>
-      <c r="K216" s="1"/>
+      <c r="K216" s="1">
+        <v>9275</v>
+      </c>
       <c r="L216" s="1"/>
-      <c r="M216" s="1"/>
+      <c r="M216" s="1">
+        <v>2</v>
+      </c>
       <c r="N216" s="1"/>
-      <c r="O216" s="1" t="str">
+      <c r="O216" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>2000---clinton.md</v>
-      </c>
-      <c r="P216" s="6"/>
-      <c r="Q216" s="6"/>
+        <v>2000-1-27-clinton.md</v>
+      </c>
+      <c r="P216" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q216" s="6" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
@@ -12018,15 +12488,15 @@
         <v>1</v>
       </c>
       <c r="N217" s="1"/>
-      <c r="O217" s="1" t="str">
+      <c r="O217" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2001-2-27-bush.md</v>
       </c>
       <c r="P217" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q217" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="Q217" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.25">
@@ -12064,15 +12534,15 @@
         <v>1</v>
       </c>
       <c r="N218" s="1"/>
-      <c r="O218" s="1" t="str">
+      <c r="O218" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2002-1-29-bush.md</v>
       </c>
       <c r="P218" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q218" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="Q218" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.25">
@@ -12110,15 +12580,15 @@
         <v>1</v>
       </c>
       <c r="N219" s="1"/>
-      <c r="O219" s="1" t="str">
+      <c r="O219" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2003-1-28-bush.md</v>
       </c>
       <c r="P219" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q219" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="Q219" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.25">
@@ -12156,15 +12626,15 @@
         <v>1</v>
       </c>
       <c r="N220" s="1"/>
-      <c r="O220" s="1" t="str">
+      <c r="O220" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2004-1-20-bush.md</v>
       </c>
       <c r="P220" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q220" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="Q220" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.25">
@@ -12202,15 +12672,15 @@
         <v>2</v>
       </c>
       <c r="N221" s="1"/>
-      <c r="O221" s="1" t="str">
+      <c r="O221" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2005-2-2-bush.md</v>
       </c>
       <c r="P221" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q221" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="Q221" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.25">
@@ -12248,15 +12718,15 @@
         <v>2</v>
       </c>
       <c r="N222" s="1"/>
-      <c r="O222" s="1" t="str">
+      <c r="O222" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2006-1-31-bush.md</v>
       </c>
       <c r="P222" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q222" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="Q222" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.25">
@@ -12294,15 +12764,15 @@
         <v>2</v>
       </c>
       <c r="N223" s="1"/>
-      <c r="O223" s="1" t="str">
+      <c r="O223" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2007-1-23-bush.md</v>
       </c>
       <c r="P223" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q223" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="Q223" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.25">
@@ -12340,15 +12810,15 @@
         <v>2</v>
       </c>
       <c r="N224" s="1"/>
-      <c r="O224" s="1" t="str">
+      <c r="O224" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2008-1-28-bush.md</v>
       </c>
       <c r="P224" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q224" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="Q224" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.25">
@@ -12386,15 +12856,15 @@
         <v>1</v>
       </c>
       <c r="N225" s="1"/>
-      <c r="O225" s="1" t="str">
+      <c r="O225" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2009-2-24-obama.md</v>
       </c>
       <c r="P225" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q225" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="Q225" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.25">
@@ -12432,15 +12902,15 @@
         <v>1</v>
       </c>
       <c r="N226" s="1"/>
-      <c r="O226" s="1" t="str">
+      <c r="O226" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2010-1-27-obama.md</v>
       </c>
       <c r="P226" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q226" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="Q226" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.25">
@@ -12478,15 +12948,15 @@
         <v>1</v>
       </c>
       <c r="N227" s="1"/>
-      <c r="O227" s="1" t="str">
+      <c r="O227" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2011-1-25-obama.md</v>
       </c>
       <c r="P227" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q227" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.25">
@@ -12524,15 +12994,15 @@
         <v>1</v>
       </c>
       <c r="N228" s="1"/>
-      <c r="O228" s="1" t="str">
+      <c r="O228" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2012-1-24-obama.md</v>
       </c>
       <c r="P228" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q228" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="229" spans="1:17" x14ac:dyDescent="0.25">
@@ -12570,15 +13040,15 @@
         <v>2</v>
       </c>
       <c r="N229" s="1"/>
-      <c r="O229" s="1" t="str">
+      <c r="O229" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2013-2-12-obama.md</v>
       </c>
       <c r="P229" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q229" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="Q229" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.25">
@@ -12616,15 +13086,15 @@
         <v>2</v>
       </c>
       <c r="N230" s="1"/>
-      <c r="O230" s="1" t="str">
+      <c r="O230" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2014-1-28-obama.md</v>
       </c>
       <c r="P230" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="231" spans="1:17" x14ac:dyDescent="0.25">
@@ -12662,7 +13132,7 @@
         <v>2</v>
       </c>
       <c r="N231" s="1"/>
-      <c r="O231" s="1" t="str">
+      <c r="O231" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2015-1-20-obama.md</v>
       </c>
@@ -12708,15 +13178,15 @@
         <v>2</v>
       </c>
       <c r="N232" s="1"/>
-      <c r="O232" s="1" t="str">
+      <c r="O232" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2016-1-12-obama.md</v>
       </c>
       <c r="P232" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q232" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="Q232" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.25">
@@ -12754,15 +13224,15 @@
         <v>1</v>
       </c>
       <c r="N233" s="1"/>
-      <c r="O233" s="1" t="str">
+      <c r="O233" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2017-2-28-trump.md</v>
       </c>
       <c r="P233" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q233" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="Q233" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -12812,7 +13282,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12849,40 +13319,40 @@
         <v>161</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -12967,7 +13437,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -12981,7 +13451,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -13014,216 +13484,263 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
       </c>
+      <c r="C33" t="s">
+        <v>233</v>
+      </c>
       <c r="D33">
         <v>1932</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>79</v>
       </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
       <c r="D35">
         <v>1952</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>82</v>
       </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
       <c r="D36">
         <v>1960</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
       </c>
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
       <c r="D37" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>85</v>
       </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
       <c r="D38">
         <v>1968</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>90</v>
       </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
       <c r="D40">
         <v>1976</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
       <c r="D41">
         <v>1980</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
+      <c r="C42" t="s">
+        <v>230</v>
+      </c>
       <c r="D42">
         <v>1988</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
       <c r="D43">
         <v>1992</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f>AVERAGE(master!K209:K216)</f>
+        <v>7713.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
       <c r="D44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f>AVERAGE(master!K217:K224)</f>
+        <v>5117.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -13236,8 +13753,12 @@
       <c r="D45">
         <v>2008</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f>AVERAGE(master!K225:K232)</f>
+        <v>6953.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
various updates/cleanup. new req's.md; R now outputs graphs to png files
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52885C4-AB74-42BE-BE64-82DB2801E962}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB15FF9-D544-4AFA-AFEA-E0978054F011}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="3" r:id="rId1"/>
@@ -28,8 +28,426 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="N217" authorId="0" shapeId="0" xr:uid="{9B81F6C1-FABB-416C-85EB-8838CA21B262}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d32</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N218" authorId="0" shapeId="0" xr:uid="{2E0ABCD4-C746-4BD7-8F09-64D5AA2F65EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d372</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N219" authorId="0" shapeId="0" xr:uid="{DF47013E-20F9-40A4-963E-DC8D51768234}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d735</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N220" authorId="0" shapeId="0" xr:uid="{2189D527-021F-4860-9018-2DA830B09FDF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1090</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N221" authorId="0" shapeId="0" xr:uid="{A683E6D6-6861-4CAD-8AE0-81A115CE566C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1457</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N222" authorId="0" shapeId="0" xr:uid="{6AF86912-8B42-4AB1-BFB9-6A922A0D4FDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1828</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N223" authorId="0" shapeId="0" xr:uid="{89DAC9E4-6083-4AC8-A9CD-86FD9B61EF56}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d2189</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N224" authorId="0" shapeId="0" xr:uid="{5F997944-3F06-41FA-AA8C-4CCA5E662FDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d2549</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N225" authorId="0" shapeId="0" xr:uid="{0FC1F798-4B1F-4BEB-A445-B1AEADB33A2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d33</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N226" authorId="0" shapeId="0" xr:uid="{30CE7D3A-6ABD-4191-A76C-ED359C78EA0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d369</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N227" authorId="0" shapeId="0" xr:uid="{19336D61-F983-47A8-92B7-EB28D0827E9B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d733</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N228" authorId="0" shapeId="0" xr:uid="{889BBB48-C8FD-4943-AB9B-BBEBC697D809}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1097</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N229" authorId="0" shapeId="0" xr:uid="{129E6B8E-85B1-4133-8518-E3D5F71BF09B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1482</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N230" authorId="0" shapeId="0" xr:uid="{0CA86425-9AA6-4060-BA06-8CFA3575F168}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d1832</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N231" authorId="0" shapeId="0" xr:uid="{021F3ECE-5051-4FD7-902F-040D54940CED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d2189</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N232" authorId="0" shapeId="0" xr:uid="{88CF4AA1-B470-489C-8082-CB11DC2A4FD3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d2546</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N233" authorId="0" shapeId="0" xr:uid="{8646A2AB-20FC-439F-8F0D-01EDFB46D06F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+d37</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="267">
   <si>
     <t>potusLastName</t>
   </si>
@@ -810,6 +1228,30 @@
   </si>
   <si>
     <t>Ronald Reagan, Address Before a Joint Session of Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/255154</t>
+  </si>
+  <si>
+    <t>POTUS approval ratings</t>
+  </si>
+  <si>
+    <t>https://news.gallup.com/interactives/185273/presidential-job-approval-center.aspx</t>
+  </si>
+  <si>
+    <t>calculate days between inauguration and SOTU. Find the nearest data point before this number of "days in office" on the Gallup chart.</t>
+  </si>
+  <si>
+    <t>word counts</t>
+  </si>
+  <si>
+    <t>https://atom.io/packages/wordcount</t>
+  </si>
+  <si>
+    <t>run as package in Atom</t>
+  </si>
+  <si>
+    <t>https://www.timeanddate.com/date/durationresult.html</t>
+  </si>
+  <si>
+    <t>to calculate days duration into term for approval ratings</t>
   </si>
 </sst>
 </file>
@@ -820,7 +1262,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,6 +1306,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -897,11 +1360,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -916,14 +1380,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="164" formatCode="00"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -942,7 +1424,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -969,6 +1451,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1022,79 +1505,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1355,6 +1766,62 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="00"/>
     </dxf>
     <dxf>
       <font>
@@ -4333,32 +4800,32 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:Q233" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="15" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="4"/>
     <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="3">
       <calculatedColumnFormula>(A2&amp;"-"&amp;B2&amp;"-"&amp;C2&amp;"-"&amp;LOWER(D2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:R46" xr:uid="{AE285793-CB7D-40A8-B930-00C5755BFACC}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6244E28B-E0F1-47FA-8860-B6D17C3A5B62}" name="#"/>
@@ -4686,11 +5153,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
   <dimension ref="A1:Q233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="M197" sqref="M197"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="M196" sqref="M196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12487,7 +12954,9 @@
       <c r="M217" s="1">
         <v>1</v>
       </c>
-      <c r="N217" s="1"/>
+      <c r="N217" s="1">
+        <v>62</v>
+      </c>
       <c r="O217" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2001-2-27-bush.md</v>
@@ -12533,7 +13002,9 @@
       <c r="M218" s="1">
         <v>1</v>
       </c>
-      <c r="N218" s="1"/>
+      <c r="N218" s="1">
+        <v>84</v>
+      </c>
       <c r="O218" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2002-1-29-bush.md</v>
@@ -12579,7 +13050,9 @@
       <c r="M219" s="1">
         <v>1</v>
       </c>
-      <c r="N219" s="1"/>
+      <c r="N219" s="1">
+        <v>60</v>
+      </c>
       <c r="O219" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2003-1-28-bush.md</v>
@@ -12625,7 +13098,9 @@
       <c r="M220" s="1">
         <v>1</v>
       </c>
-      <c r="N220" s="1"/>
+      <c r="N220" s="1">
+        <v>53</v>
+      </c>
       <c r="O220" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2004-1-20-bush.md</v>
@@ -12671,7 +13146,9 @@
       <c r="M221" s="1">
         <v>2</v>
       </c>
-      <c r="N221" s="1"/>
+      <c r="N221" s="1">
+        <v>51</v>
+      </c>
       <c r="O221" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2005-2-2-bush.md</v>
@@ -12717,7 +13194,9 @@
       <c r="M222" s="1">
         <v>2</v>
       </c>
-      <c r="N222" s="1"/>
+      <c r="N222" s="1">
+        <v>43</v>
+      </c>
       <c r="O222" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2006-1-31-bush.md</v>
@@ -12763,7 +13242,9 @@
       <c r="M223" s="1">
         <v>2</v>
       </c>
-      <c r="N223" s="1"/>
+      <c r="N223" s="1">
+        <v>36</v>
+      </c>
       <c r="O223" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2007-1-23-bush.md</v>
@@ -12809,7 +13290,9 @@
       <c r="M224" s="1">
         <v>2</v>
       </c>
-      <c r="N224" s="1"/>
+      <c r="N224" s="1">
+        <v>34</v>
+      </c>
       <c r="O224" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2008-1-28-bush.md</v>
@@ -12855,7 +13338,9 @@
       <c r="M225" s="1">
         <v>1</v>
       </c>
-      <c r="N225" s="1"/>
+      <c r="N225" s="1">
+        <v>62</v>
+      </c>
       <c r="O225" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2009-2-24-obama.md</v>
@@ -12901,7 +13386,9 @@
       <c r="M226" s="1">
         <v>1</v>
       </c>
-      <c r="N226" s="1"/>
+      <c r="N226" s="1">
+        <v>49</v>
+      </c>
       <c r="O226" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2010-1-27-obama.md</v>
@@ -12947,7 +13434,9 @@
       <c r="M227" s="1">
         <v>1</v>
       </c>
-      <c r="N227" s="1"/>
+      <c r="N227" s="1">
+        <v>50</v>
+      </c>
       <c r="O227" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2011-1-25-obama.md</v>
@@ -12993,7 +13482,9 @@
       <c r="M228" s="1">
         <v>1</v>
       </c>
-      <c r="N228" s="1"/>
+      <c r="N228" s="1">
+        <v>45</v>
+      </c>
       <c r="O228" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2012-1-24-obama.md</v>
@@ -13039,7 +13530,9 @@
       <c r="M229" s="1">
         <v>2</v>
       </c>
-      <c r="N229" s="1"/>
+      <c r="N229" s="1">
+        <v>52</v>
+      </c>
       <c r="O229" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2013-2-12-obama.md</v>
@@ -13085,7 +13578,9 @@
       <c r="M230" s="1">
         <v>2</v>
       </c>
-      <c r="N230" s="1"/>
+      <c r="N230" s="1">
+        <v>42</v>
+      </c>
       <c r="O230" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2014-1-28-obama.md</v>
@@ -13131,7 +13626,9 @@
       <c r="M231" s="1">
         <v>2</v>
       </c>
-      <c r="N231" s="1"/>
+      <c r="N231" s="1">
+        <v>46</v>
+      </c>
       <c r="O231" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2015-1-20-obama.md</v>
@@ -13177,7 +13674,9 @@
       <c r="M232" s="1">
         <v>2</v>
       </c>
-      <c r="N232" s="1"/>
+      <c r="N232" s="1">
+        <v>47</v>
+      </c>
       <c r="O232" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2016-1-12-obama.md</v>
@@ -13223,7 +13722,9 @@
       <c r="M233" s="1">
         <v>1</v>
       </c>
-      <c r="N233" s="1"/>
+      <c r="N233" s="1">
+        <v>42</v>
+      </c>
       <c r="O233" s="13" t="str">
         <f t="shared" si="3"/>
         <v>2017-2-28-trump.md</v>
@@ -13247,8 +13748,9 @@
   <ignoredErrors>
     <ignoredError sqref="B1:C1" listDataValidation="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -13282,7 +13784,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13735,6 +14237,9 @@
       <c r="D44">
         <v>2000</v>
       </c>
+      <c r="E44" s="14">
+        <v>36911</v>
+      </c>
       <c r="G44">
         <f>AVERAGE(master!K217:K224)</f>
         <v>5117.625</v>
@@ -13753,6 +14258,9 @@
       <c r="D45">
         <v>2008</v>
       </c>
+      <c r="E45" s="14">
+        <v>39833</v>
+      </c>
       <c r="G45">
         <f>AVERAGE(master!K225:K232)</f>
         <v>6953.75</v>
@@ -13770,6 +14278,9 @@
       </c>
       <c r="D46">
         <v>2016</v>
+      </c>
+      <c r="E46" s="14">
+        <v>42755</v>
       </c>
     </row>
   </sheetData>
@@ -13782,19 +14293,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EBFBCF-E6C2-4EF0-9842-2DFDC52BE682}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="128.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -13802,7 +14314,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -13810,7 +14322,41 @@
         <v>97</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{FBBFBDF0-F1E0-474A-9F78-15BAF6DD0EF3}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{0A2F2999-CEE5-4F04-9A6B-A4678D0FA624}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added 2018 and 2019 texts, updated master index
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1293746-C414-4240-A5FC-67F677CAC9C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3230E2F8-FED2-444F-9033-17B3557DB36E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -448,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="301">
   <si>
     <t>potusLastName</t>
   </si>
@@ -1346,6 +1345,24 @@
   </si>
   <si>
     <t>Jimmy Carter, The State of the Union Annual Message to the Congress Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/245130</t>
+  </si>
+  <si>
+    <t>Delayed due to shutdown/Nancy Pelosi</t>
+  </si>
+  <si>
+    <t>2019-02-05-trump.md</t>
+  </si>
+  <si>
+    <t>Donald J. Trump, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/332430</t>
+  </si>
+  <si>
+    <t>NOTE: This is a transcript of the remarks a prepared for delivery.  A transcript of the remarks as delivered will be posted once it is available.</t>
+  </si>
+  <si>
+    <t>Begins with the words "The President." in italics, omitted from .md file.   NOTE: The President spoke at 9:10 p.m. in the House Chamber of the U.S. Capitol. In his remarks, he referred to Supreme Court Associate Justice Neil M. Gorsuch; Alexi Saenz, Jairo Saenz, Selvin Chavez, and Enrique Portillo, who, along with two unnamed minors, are accused in the murder of Brentwood, NY, residents Kayla Cuevas and Nisa Mickens in Brentwood on September 13, 2016; Crystal Champ, birth mother of Hope Holets; and Abu Bakr al-Baghdadi, leader of the Islamic State of Iraq and Syria (ISIS) terrorist organization. He also referred to Executive Order 13823.</t>
+  </si>
+  <si>
+    <t>Donald J. Trump, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/331779</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1476,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1481,6 +1498,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1488,144 +1506,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1987,6 +1867,114 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -2040,6 +2028,36 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2382,7 +2400,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>132</c:v>
@@ -2716,10 +2734,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>master!$B$2:$B$236</c:f>
+              <c:f>master!$B$2:$B$238</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="235"/>
+                <c:ptCount val="237"/>
                 <c:pt idx="0">
                   <c:v>1790</c:v>
                 </c:pt>
@@ -3424,16 +3442,22 @@
                 </c:pt>
                 <c:pt idx="234">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="235" formatCode="00">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="236" formatCode="00">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>master!$L$2:$L$236</c:f>
+              <c:f>master!$L$2:$L$238</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="235"/>
+                <c:ptCount val="237"/>
                 <c:pt idx="0">
                   <c:v>1089</c:v>
                 </c:pt>
@@ -3685,6 +3709,12 @@
                 </c:pt>
                 <c:pt idx="234">
                   <c:v>5089</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>5828</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>5249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5096,35 +5126,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:R236" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:R237" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <tableColumns count="18">
-    <tableColumn id="12" xr3:uid="{724596CD-E5E0-4C9C-9CE9-2CB5DFDA8FDE}" name="sotuid" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="18"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="12">
+    <tableColumn id="12" xr3:uid="{724596CD-E5E0-4C9C-9CE9-2CB5DFDA8FDE}" name="sotuid" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="2">
       <calculatedColumnFormula>(B2&amp;"-"&amp;C2&amp;"-"&amp;D2&amp;"-"&amp;LOWER(E2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A1:R46" xr:uid="{AE285793-CB7D-40A8-B930-00C5755BFACC}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6244E28B-E0F1-47FA-8860-B6D17C3A5B62}" name="#"/>
@@ -5175,17 +5205,17 @@
   <autoFilter ref="E1:F13" xr:uid="{5E0E19EC-E787-4E95-B2A0-DA3101E4B9CA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{13B4AD1F-1158-4533-9B2D-9CFE591E304C}" name="Months"/>
-    <tableColumn id="2" xr3:uid="{C8A49BA1-4372-41EE-98D0-74E91D22AEE1}" name="Column1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C8A49BA1-4372-41EE-98D0-74E91D22AEE1}" name="Column1" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E0C97C5F-B132-4DCF-A62A-D236753529D9}" name="Table6" displayName="Table6" ref="G1:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E0C97C5F-B132-4DCF-A62A-D236753529D9}" name="Table6" displayName="Table6" ref="G1:G32" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="G1:G32" xr:uid="{CB8F412D-685E-443A-B695-BC1012C614D8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D5A23D3D-381F-4AC0-924E-FD70DC3BB239}" name="Dates" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{D5A23D3D-381F-4AC0-924E-FD70DC3BB239}" name="Dates" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5454,10 +5484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
-  <dimension ref="A1:R236"/>
+  <dimension ref="A1:R238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D182" workbookViewId="0">
-      <selection activeCell="Q196" sqref="Q196"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S243" sqref="S243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13283,7 +13314,7 @@
       </c>
       <c r="O197" s="17"/>
       <c r="P197" s="13" t="str">
-        <f t="shared" ref="P197:P198" si="3">(B197&amp;"-"&amp;C197&amp;"-"&amp;D197&amp;"-"&amp;LOWER(E197)&amp;".md")</f>
+        <f t="shared" ref="P197" si="3">(B197&amp;"-"&amp;C197&amp;"-"&amp;D197&amp;"-"&amp;LOWER(E197)&amp;".md")</f>
         <v>1980-01-21-carter.md</v>
       </c>
       <c r="Q197" s="6" t="s">
@@ -15238,12 +15269,109 @@
         <v>196</v>
       </c>
     </row>
+    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>236</v>
+      </c>
+      <c r="B237" s="21">
+        <v>2018</v>
+      </c>
+      <c r="C237" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D237" s="19">
+        <v>30</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G237" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H237" s="1"/>
+      <c r="I237" s="1">
+        <v>1</v>
+      </c>
+      <c r="J237" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K237" s="1"/>
+      <c r="L237" s="1">
+        <v>5828</v>
+      </c>
+      <c r="M237" s="1"/>
+      <c r="N237" s="1">
+        <v>1</v>
+      </c>
+      <c r="O237" s="17"/>
+      <c r="P237" s="13" t="str">
+        <f>(B237&amp;"-"&amp;C237&amp;"-"&amp;D237&amp;"-"&amp;LOWER(E237)&amp;".md")</f>
+        <v>2018-01-30-trump.md</v>
+      </c>
+      <c r="Q237" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="R237" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D238" t="s">
+        <v>271</v>
+      </c>
+      <c r="E238" t="s">
+        <v>9</v>
+      </c>
+      <c r="F238" t="s">
+        <v>95</v>
+      </c>
+      <c r="G238" t="s">
+        <v>17</v>
+      </c>
+      <c r="H238" t="s">
+        <v>295</v>
+      </c>
+      <c r="I238">
+        <v>1</v>
+      </c>
+      <c r="J238" t="s">
+        <v>108</v>
+      </c>
+      <c r="L238">
+        <v>5249</v>
+      </c>
+      <c r="N238">
+        <v>1</v>
+      </c>
+      <c r="P238" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q238" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="R238" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C1 B237:B1048576" xr:uid="{DB144446-EB57-47C0-BE17-4F8D925A6CFF}">
+  <dataValidations count="2">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C1 B239:B1048576" xr:uid="{DB144446-EB57-47C0-BE17-4F8D925A6CFF}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B237:B238" xr:uid="{5C2D0870-597B-4AEA-B4C2-D6111C8831CE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15262,25 +15390,25 @@
           <x14:formula1>
             <xm:f>vocabulary!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G236</xm:sqref>
+          <xm:sqref>G2:G237</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF5FC0A3-8F38-4D54-BB5D-B7B2956A0A1B}">
           <x14:formula1>
             <xm:f>vocabulary!$C$2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:K236</xm:sqref>
+          <xm:sqref>J1:K237</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{BD3C8EC6-B7A2-4480-9675-99CF90A83F22}">
           <x14:formula1>
             <xm:f>vocabulary!$F$2:$F$13</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C236</xm:sqref>
+          <xm:sqref>C2:C236 C237:C238</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{863E898A-9393-44B1-82F7-419B3770C50E}">
           <x14:formula1>
             <xm:f>vocabulary!$G$2:$G$32</xm:f>
           </x14:formula1>
-          <xm:sqref>C237:C1048576 D1:D236</xm:sqref>
+          <xm:sqref>C239:C1048576 D1:D236 D237:D238</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15874,8 +16002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DDDDA2-CD65-4F05-8376-3F7C0FDAE546}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15889,7 +16017,7 @@
       </c>
       <c r="B1">
         <f>COUNTA(Table3[deliveredYear])</f>
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -15902,8 +16030,8 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(master!G2:G236,vocabulary!A3)</f>
-        <v>100</v>
+        <f>COUNTIF(master!G2:G237,vocabulary!A3)</f>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -15911,7 +16039,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(master!G2:G236,vocabulary!A2)</f>
+        <f>COUNTIF(master!G2:G237,vocabulary!A2)</f>
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated 2019 sotu to "as delivered," created seperate file for "as prepared."
</commit_message>
<xml_diff>
--- a/master-index.xlsx
+++ b/master-index.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3230E2F8-FED2-444F-9033-17B3557DB36E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB128E-C261-4FDB-BCF7-CF10C3A3C762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="302">
   <si>
     <t>potusLastName</t>
   </si>
@@ -1350,19 +1350,22 @@
     <t>Delayed due to shutdown/Nancy Pelosi</t>
   </si>
   <si>
-    <t>2019-02-05-trump.md</t>
-  </si>
-  <si>
     <t>Donald J. Trump, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/332430</t>
   </si>
   <si>
-    <t>NOTE: This is a transcript of the remarks a prepared for delivery.  A transcript of the remarks as delivered will be posted once it is available.</t>
-  </si>
-  <si>
     <t>Begins with the words "The President." in italics, omitted from .md file.   NOTE: The President spoke at 9:10 p.m. in the House Chamber of the U.S. Capitol. In his remarks, he referred to Supreme Court Associate Justice Neil M. Gorsuch; Alexi Saenz, Jairo Saenz, Selvin Chavez, and Enrique Portillo, who, along with two unnamed minors, are accused in the murder of Brentwood, NY, residents Kayla Cuevas and Nisa Mickens in Brentwood on September 13, 2016; Crystal Champ, birth mother of Hope Holets; and Abu Bakr al-Baghdadi, leader of the Islamic State of Iraq and Syria (ISIS) terrorist organization. He also referred to Executive Order 13823.</t>
   </si>
   <si>
     <t>Donald J. Trump, Address Before a Joint Session of the Congress on the State of the Union Online by Gerhard Peters and John T. Woolley, The American Presidency Project https://www.presidency.ucsb.edu/node/331779</t>
+  </si>
+  <si>
+    <t>NOTE: This is a transcript of the remarks a prepared for delivery.</t>
+  </si>
+  <si>
+    <t>2019 SOTU as prepared for deliverY</t>
+  </si>
+  <si>
+    <t>2019-02-05-trump--as-prepared.md</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1442,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1452,8 +1455,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1470,13 +1479,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1499,6 +1519,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1506,6 +1527,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2029,36 +2080,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2400,7 +2421,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>101</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>132</c:v>
@@ -2734,10 +2755,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>master!$B$2:$B$238</c:f>
+              <c:f>master!$B$2:$B$239</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="237"/>
+                <c:ptCount val="238"/>
                 <c:pt idx="0">
                   <c:v>1790</c:v>
                 </c:pt>
@@ -3447,6 +3468,9 @@
                   <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="236" formatCode="00">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="237" formatCode="00">
                   <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
@@ -3454,10 +3478,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>master!$L$2:$L$238</c:f>
+              <c:f>master!$L$2:$L$239</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="237"/>
+                <c:ptCount val="238"/>
                 <c:pt idx="0">
                   <c:v>1089</c:v>
                 </c:pt>
@@ -3714,6 +3738,9 @@
                   <c:v>5828</c:v>
                 </c:pt>
                 <c:pt idx="236">
+                  <c:v>5723</c:v>
+                </c:pt>
+                <c:pt idx="237">
                   <c:v>5249</c:v>
                 </c:pt>
               </c:numCache>
@@ -5126,35 +5153,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:R237" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD1BD357-B2E9-449F-8260-5EBC10B7E30B}" name="Table3" displayName="Table3" ref="A1:R238" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <tableColumns count="18">
-    <tableColumn id="12" xr3:uid="{724596CD-E5E0-4C9C-9CE9-2CB5DFDA8FDE}" name="sotuid" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{724596CD-E5E0-4C9C-9CE9-2CB5DFDA8FDE}" name="sotuid" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{7B1541F7-1420-499B-84B0-DDBCE30A6B9F}" name="deliveredYear" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E5DA78A8-D8EC-4D94-9182-115EC7E12A0A}" name="deliveredMonth" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{BABAE1A0-DDCA-4D7F-88A1-65C21D264FB2}" name="deliveredDate" dataDxfId="19" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C32B71B8-877D-4AE3-907F-792C10C6D836}" name="potusLastName" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{62A98585-9D59-472F-BE4A-CC3781D4ECE8}" name="potusGivenNames" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{3A028ED7-9126-45CD-8215-829006454653}" name="deliveryMedium" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{62A40F6A-36E6-45DD-9E9A-C150022D0158}" name="specialDelivery" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{32316ED5-DCA4-4B8C-8FB7-80B629FC8A2A}" name="isSOTU" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{41CF975F-B342-43DE-8A0A-CDB1158AF583}" name="potusParty" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{AD03A8C2-7013-424B-B7D6-F4841933513F}" name="potusParty2" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{2D67A190-84D8-4575-A4B4-EB96EAF062DC}" name="sotuWordCount" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{AF90EB0F-6682-4B57-8072-C303CF34CAAD}" name="monthsInOffice" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{1EE15E54-3F5A-4E8F-84BB-7C4A4CFACEA8}" name="potusTerm" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{595425A0-FD4B-4503-9E76-4DEF78C55A2C}" name="approvalRating" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{C0C3B4D1-5601-4DBB-B6EF-4D50C83BB51C}" name="ucsb-filename" dataDxfId="7">
       <calculatedColumnFormula>(B2&amp;"-"&amp;C2&amp;"-"&amp;D2&amp;"-"&amp;LOWER(E2)&amp;".md")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{1AE66F0D-C3F9-4BFD-AB7B-22D81EE8B3A9}" name="ucsb-comments" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{26C47F06-6E20-4518-94F9-0AAE8B3855C4}" name="ucsb-citation" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2165DEDF-1AB7-4B84-9632-A614CDA07411}" name="Table1" displayName="Table1" ref="A1:R46" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:R46" xr:uid="{AE285793-CB7D-40A8-B930-00C5755BFACC}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6244E28B-E0F1-47FA-8860-B6D17C3A5B62}" name="#"/>
@@ -5205,17 +5232,17 @@
   <autoFilter ref="E1:F13" xr:uid="{5E0E19EC-E787-4E95-B2A0-DA3101E4B9CA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{13B4AD1F-1158-4533-9B2D-9CFE591E304C}" name="Months"/>
-    <tableColumn id="2" xr3:uid="{C8A49BA1-4372-41EE-98D0-74E91D22AEE1}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{C8A49BA1-4372-41EE-98D0-74E91D22AEE1}" name="Column1" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E0C97C5F-B132-4DCF-A62A-D236753529D9}" name="Table6" displayName="Table6" ref="G1:G32" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E0C97C5F-B132-4DCF-A62A-D236753529D9}" name="Table6" displayName="Table6" ref="G1:G32" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="G1:G32" xr:uid="{CB8F412D-685E-443A-B695-BC1012C614D8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D5A23D3D-381F-4AC0-924E-FD70DC3BB239}" name="Dates" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{D5A23D3D-381F-4AC0-924E-FD70DC3BB239}" name="Dates" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5484,11 +5511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15899E-558C-4C63-B86C-F370C964819B}">
-  <dimension ref="A1:R238"/>
+  <dimension ref="A1:R239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S243" sqref="S243"/>
+      <selection pane="bottomLeft" activeCell="Q242" sqref="Q242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15312,66 +15339,109 @@
         <v>2018-01-30-trump.md</v>
       </c>
       <c r="Q237" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R237" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A238">
+      <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="9">
+      <c r="B238" s="21">
         <v>2019</v>
       </c>
-      <c r="C238" s="4" t="s">
+      <c r="C238" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E238" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F238" t="s">
+      <c r="F238" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G238" t="s">
+      <c r="G238" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H238" t="s">
         <v>295</v>
       </c>
-      <c r="I238">
-        <v>1</v>
-      </c>
-      <c r="J238" t="s">
+      <c r="I238" s="1">
+        <v>1</v>
+      </c>
+      <c r="J238" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L238">
+      <c r="K238" s="1"/>
+      <c r="L238" s="1">
+        <v>5723</v>
+      </c>
+      <c r="M238" s="1"/>
+      <c r="N238" s="1">
+        <v>1</v>
+      </c>
+      <c r="O238" s="17"/>
+      <c r="P238" s="13" t="str">
+        <f>(B238&amp;"-"&amp;C238&amp;"-"&amp;D238&amp;"-"&amp;LOWER(E238)&amp;".md")</f>
+        <v>2019-02-05-trump.md</v>
+      </c>
+      <c r="Q238" s="6"/>
+      <c r="R238" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D239" t="s">
+        <v>271</v>
+      </c>
+      <c r="E239" t="s">
+        <v>9</v>
+      </c>
+      <c r="F239" t="s">
+        <v>95</v>
+      </c>
+      <c r="G239" t="s">
+        <v>17</v>
+      </c>
+      <c r="H239" t="s">
+        <v>300</v>
+      </c>
+      <c r="J239" t="s">
+        <v>108</v>
+      </c>
+      <c r="L239">
         <v>5249</v>
       </c>
-      <c r="N238">
-        <v>1</v>
-      </c>
-      <c r="P238" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q238" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="R238" s="3" t="s">
-        <v>297</v>
+      <c r="N239">
+        <v>1</v>
+      </c>
+      <c r="P239" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q239" s="22" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C1 B239:B1048576" xr:uid="{DB144446-EB57-47C0-BE17-4F8D925A6CFF}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C1 B240:B1048576" xr:uid="{DB144446-EB57-47C0-BE17-4F8D925A6CFF}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B237:B238" xr:uid="{5C2D0870-597B-4AEA-B4C2-D6111C8831CE}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B237:B239" xr:uid="{5C2D0870-597B-4AEA-B4C2-D6111C8831CE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15390,25 +15460,25 @@
           <x14:formula1>
             <xm:f>vocabulary!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G237</xm:sqref>
+          <xm:sqref>G2:G238</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF5FC0A3-8F38-4D54-BB5D-B7B2956A0A1B}">
           <x14:formula1>
             <xm:f>vocabulary!$C$2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:K237</xm:sqref>
+          <xm:sqref>J1:K238</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{BD3C8EC6-B7A2-4480-9675-99CF90A83F22}">
           <x14:formula1>
             <xm:f>vocabulary!$F$2:$F$13</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C236 C237:C238</xm:sqref>
+          <xm:sqref>C2:C239</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{863E898A-9393-44B1-82F7-419B3770C50E}">
           <x14:formula1>
             <xm:f>vocabulary!$G$2:$G$32</xm:f>
           </x14:formula1>
-          <xm:sqref>C239:C1048576 D1:D236 D237:D238</xm:sqref>
+          <xm:sqref>C240:C1048576 D1:D239</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -16017,7 +16087,7 @@
       </c>
       <c r="B1">
         <f>COUNTA(Table3[deliveredYear])</f>
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -16030,8 +16100,8 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(master!G2:G237,vocabulary!A3)</f>
-        <v>101</v>
+        <f>COUNTIF(master!G2:G238,vocabulary!A3)</f>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -16039,7 +16109,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(master!G2:G237,vocabulary!A2)</f>
+        <f>COUNTIF(master!G2:G238,vocabulary!A2)</f>
         <v>132</v>
       </c>
     </row>

</xml_diff>